<commit_message>
:rocket: Update vom 03.03.2023
</commit_message>
<xml_diff>
--- a/Kontrolle Noten und Anwesenheit_Template.xlsx
+++ b/Kontrolle Noten und Anwesenheit_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://baumgartnerrhf.sharepoint.com/sites/hfict/Freigegebene Dokumente/Allgemein/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://baumgartnerrhf.sharepoint.com/sites/hfict/Freigegebene Dokumente/01 Allgemeine Informationen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1683" documentId="13_ncr:1_{E46A93A5-8711-4C71-8FC9-6D0FE0D618DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{842E6E5B-ADDD-4C14-9A50-560E74A34566}"/>
+  <xr:revisionPtr revIDLastSave="1694" documentId="13_ncr:1_{E46A93A5-8711-4C71-8FC9-6D0FE0D618DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18D3787B-B815-4333-A5CF-0F644F262D75}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0EC385B7-3D0C-45EA-864E-7EE127AA989A}"/>
+    <workbookView xWindow="20235" yWindow="3600" windowWidth="26325" windowHeight="19110" xr2:uid="{0EC385B7-3D0C-45EA-864E-7EE127AA989A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hauptübersicht" sheetId="3" r:id="rId1"/>
@@ -1512,6 +1512,21 @@
   </cellStyles>
   <dxfs count="161">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="medium">
@@ -1671,9 +1686,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1681,9 +1693,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -1854,9 +1863,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2025,9 +2031,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2267,9 +2270,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2478,10 +2478,10 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{0B6DEAD9-1104-4ECE-96C7-96A7390E4FE0}" name="Allgemeines"/>
     <tableColumn id="2" xr3:uid="{14351AFC-7D21-4CC8-BFC0-51F07CA3F24F}" name="Fach"/>
-    <tableColumn id="3" xr3:uid="{2618ED18-84F8-40E0-89E6-DBD03E5614F0}" name="Status" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{2618ED18-84F8-40E0-89E6-DBD03E5614F0}" name="Status" dataDxfId="23"/>
     <tableColumn id="4" xr3:uid="{4A77C64F-316A-4D24-9F63-6BD4F2EA8963}" name="LLP max"/>
-    <tableColumn id="5" xr3:uid="{BE713E1B-AE97-4051-A260-5B90326948E1}" name="Note" dataDxfId="19">
-      <calculatedColumnFormula>IF(((TBL_Allgemeines[[#This Row],[LLP Total]]/(TBL_Allgemeines[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Allgemeines[[#This Row],[LLP Total]]/(TBL_Allgemeines[[#This Row],[LLP max]]*0.9)*5))</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{BE713E1B-AE97-4051-A260-5B90326948E1}" name="Note" dataDxfId="0">
+      <calculatedColumnFormula>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/((TBL_Allgemeines[[#This Row],[LLP max]]*0.6)-TBL_Allgemeines[[#This Row],[LLP max]]*0.16))*TBL_Allgemeines[[#This Row],[LLP Total]]))),2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{E357EBB0-CCB5-4DE1-BB3B-4382AD9C871D}" name="LLP Total"/>
   </tableColumns>
@@ -2495,30 +2495,30 @@
   <tableColumns count="251">
     <tableColumn id="1" xr3:uid="{89E93B22-973E-4333-9CBE-00278C4A57EE}" name="Schwerpunkt Softwareentwicklung"/>
     <tableColumn id="2" xr3:uid="{DA66D9D3-ADEF-403B-B1DD-B2B38430E08C}" name="Fach"/>
-    <tableColumn id="67" xr3:uid="{56DDF1FC-4004-4B95-B3DC-A1D43FD1305E}" name="Status" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{547BBAFA-B951-4B8A-B093-D6658A5800A6}" name="LLP max" dataDxfId="17">
+    <tableColumn id="67" xr3:uid="{56DDF1FC-4004-4B95-B3DC-A1D43FD1305E}" name="Status" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{547BBAFA-B951-4B8A-B093-D6658A5800A6}" name="LLP max" dataDxfId="21">
       <calculatedColumnFormula>VLOOKUP(TBL_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],Übersicht_Fächer!A35:E43,5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{C3B62345-03EC-4A83-9D24-82FBA79E5353}" name="Kontrolle LLP max" dataDxfId="16">
+    <tableColumn id="47" xr3:uid="{C3B62345-03EC-4A83-9D24-82FBA79E5353}" name="Kontrolle LLP max" dataDxfId="20">
       <calculatedColumnFormula>TBL_S_Software[[#This Row],[Mastery Max]]+TBL_S_Software[[#This Row],[ATL Max]]+TBL_S_Software[[#This Row],[Präsenz Max]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BF45F161-567C-49D8-89A0-85A89818A93C}" name="Note" dataDxfId="15">
-      <calculatedColumnFormula>IF(((TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5))</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{BF45F161-567C-49D8-89A0-85A89818A93C}" name="Note" dataDxfId="1">
+      <calculatedColumnFormula>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{D4002414-1F10-4958-BAAE-615B24C98835}" name="LLP Total" dataDxfId="14">
+    <tableColumn id="23" xr3:uid="{D4002414-1F10-4958-BAAE-615B24C98835}" name="LLP Total" dataDxfId="19">
       <calculatedColumnFormula>TBL_S_Software[[#This Row],[Mastery]]+TBL_S_Software[[#This Row],[ATL]]+TBL_S_Software[[#This Row],[Präsenz]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="45" xr3:uid="{590D9C15-5F06-4D49-97BC-F8AD7A30D260}" name="Mastery Max"/>
     <tableColumn id="22" xr3:uid="{CA54A5DB-9122-491B-91E6-3A0E2B5AB402}" name="Mastery"/>
     <tableColumn id="44" xr3:uid="{1681684C-779F-4005-BD82-D2A7A66DF5A3}" name="ATL Max"/>
     <tableColumn id="24" xr3:uid="{95B1017A-B935-4695-A420-B6BAC359CAC4}" name="ATL"/>
-    <tableColumn id="43" xr3:uid="{E2ED21C2-B7A2-44BF-9FEE-2A2BE7528ED3}" name="Präsenz Max" dataDxfId="13">
+    <tableColumn id="43" xr3:uid="{E2ED21C2-B7A2-44BF-9FEE-2A2BE7528ED3}" name="Präsenz Max" dataDxfId="18">
       <calculatedColumnFormula>VLOOKUP(TBL_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],Übersicht_Fächer!A35:E43,4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8E4610E4-C97D-46F5-BF40-AAFD208AF40D}" name="Präsenz" dataDxfId="12">
+    <tableColumn id="5" xr3:uid="{8E4610E4-C97D-46F5-BF40-AAFD208AF40D}" name="Präsenz" dataDxfId="17">
       <calculatedColumnFormula>SUM(TBL_S_Software[[#This Row],[01.02.2022]:[26.06.2025]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3AEB9746-ED19-48C5-8ED8-5656E9DDD8CB}" name="01.02.2022" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{3AEB9746-ED19-48C5-8ED8-5656E9DDD8CB}" name="01.02.2022" dataDxfId="16"/>
     <tableColumn id="7" xr3:uid="{DEBFDFA4-786E-434F-A3DE-01F5191C86AB}" name="03.02.2022"/>
     <tableColumn id="8" xr3:uid="{2179D8F5-C2D1-4718-9ACC-892F7F1513FA}" name="08.02.2022"/>
     <tableColumn id="9" xr3:uid="{BC6CB5BE-4858-40BF-953F-1920C7CF64EE}" name="10.02.2022"/>
@@ -2565,8 +2565,8 @@
     <tableColumn id="57" xr3:uid="{46267134-67F9-4998-B689-2DB6A06BEA1F}" name="10.01.2023"/>
     <tableColumn id="58" xr3:uid="{935543E6-F282-4F95-9BA7-03BB44BE9AB6}" name="12.01.2023"/>
     <tableColumn id="59" xr3:uid="{8D9A52DE-AAC4-4CA6-A061-6AAE718C9E82}" name="17.01.2023"/>
-    <tableColumn id="60" xr3:uid="{BE003BD5-0B89-497F-BC0F-67C59EABF23E}" name="19.01.2023" dataDxfId="10"/>
-    <tableColumn id="61" xr3:uid="{05454EA3-4F8A-4512-8417-1A188E0986D1}" name="24.01.2023" dataDxfId="9"/>
+    <tableColumn id="60" xr3:uid="{BE003BD5-0B89-497F-BC0F-67C59EABF23E}" name="19.01.2023" dataDxfId="15"/>
+    <tableColumn id="61" xr3:uid="{05454EA3-4F8A-4512-8417-1A188E0986D1}" name="24.01.2023" dataDxfId="14"/>
     <tableColumn id="62" xr3:uid="{CA61AC3D-00D8-44D8-B235-02E6B4BA2E6E}" name="26.01.2023"/>
     <tableColumn id="63" xr3:uid="{7B240D45-196D-4225-9632-811F0A528441}" name="31.01.2023"/>
     <tableColumn id="64" xr3:uid="{73F05805-6384-4018-AB2C-1EE8A6C0AC78}" name="02.02.2023"/>
@@ -2603,8 +2603,8 @@
     <tableColumn id="96" xr3:uid="{E3F46D1E-BF65-40C2-8495-D4B4D564BA7C}" name="20.06.2023"/>
     <tableColumn id="97" xr3:uid="{680A6F9F-960C-4F5C-9D69-F9292A6D44D1}" name="22.06.2023"/>
     <tableColumn id="98" xr3:uid="{E2FA3ED7-CC17-4FB1-B40E-5327A268F6E5}" name="27.06.2023"/>
-    <tableColumn id="99" xr3:uid="{BA7716BD-4259-4934-AB3F-09599A595B88}" name="29.06.2023" dataDxfId="8"/>
-    <tableColumn id="100" xr3:uid="{588FF384-94A3-48A9-8307-56E1B1A95ACA}" name="15.08.2023" dataDxfId="7"/>
+    <tableColumn id="99" xr3:uid="{BA7716BD-4259-4934-AB3F-09599A595B88}" name="29.06.2023" dataDxfId="13"/>
+    <tableColumn id="100" xr3:uid="{588FF384-94A3-48A9-8307-56E1B1A95ACA}" name="15.08.2023" dataDxfId="12"/>
     <tableColumn id="101" xr3:uid="{5680FFCE-E734-4FCE-8055-E9F762C27B3A}" name="17.08.2023"/>
     <tableColumn id="102" xr3:uid="{2F83767E-15DB-40FF-8BDC-B54AA62C6FF0}" name="22.08.2023"/>
     <tableColumn id="103" xr3:uid="{039B3B17-DEB6-4EAC-933C-CAE77E5CA960}" name="24.08.2023"/>
@@ -2641,8 +2641,8 @@
     <tableColumn id="134" xr3:uid="{B8E96AAC-44A8-4DED-8E42-3310FA3213C2}" name="09.01.2024"/>
     <tableColumn id="135" xr3:uid="{0376BE40-B54C-45AE-BB2C-B330D9EFF082}" name="11.01.2024"/>
     <tableColumn id="136" xr3:uid="{1B9B728A-992C-4762-9AB3-D6AB458F603E}" name="16.01.2024"/>
-    <tableColumn id="137" xr3:uid="{41369DF5-6A09-4A01-970D-D0402558FC04}" name="18.01.2024" dataDxfId="6"/>
-    <tableColumn id="138" xr3:uid="{8AC786F4-DB5A-4232-B7A0-19EC5381586A}" name="23.01.2024" dataDxfId="5"/>
+    <tableColumn id="137" xr3:uid="{41369DF5-6A09-4A01-970D-D0402558FC04}" name="18.01.2024" dataDxfId="11"/>
+    <tableColumn id="138" xr3:uid="{8AC786F4-DB5A-4232-B7A0-19EC5381586A}" name="23.01.2024" dataDxfId="10"/>
     <tableColumn id="139" xr3:uid="{5948E057-777F-4A07-A21C-B16159F40BA7}" name="25.01.2024"/>
     <tableColumn id="140" xr3:uid="{2DF751F1-5125-4733-A5A3-A91AB915505C}" name="30.01.2024"/>
     <tableColumn id="141" xr3:uid="{291F12C0-FF15-4712-A9C9-3BFFC4A747F6}" name="01.02.2024"/>
@@ -2679,8 +2679,8 @@
     <tableColumn id="172" xr3:uid="{C04C4065-F651-48B8-A1FD-0C3F2319198D}" name="18.06.2024"/>
     <tableColumn id="173" xr3:uid="{499207CD-E56F-42B2-AE26-83B4CE28DE4D}" name="20.06.2024"/>
     <tableColumn id="174" xr3:uid="{A4538A39-8339-47E7-A822-2A15170F0F1B}" name="25.06.2024"/>
-    <tableColumn id="175" xr3:uid="{A90CA91D-7085-47B4-B130-CCF4DDC6CE34}" name="27.06.2024" dataDxfId="4"/>
-    <tableColumn id="176" xr3:uid="{F900020A-B219-45E4-B5E6-78CAFCC213BE}" name="13.08.2024" dataDxfId="3"/>
+    <tableColumn id="175" xr3:uid="{A90CA91D-7085-47B4-B130-CCF4DDC6CE34}" name="27.06.2024" dataDxfId="9"/>
+    <tableColumn id="176" xr3:uid="{F900020A-B219-45E4-B5E6-78CAFCC213BE}" name="13.08.2024" dataDxfId="8"/>
     <tableColumn id="177" xr3:uid="{F6F6D3D4-76DD-4AF5-BE9C-5ABD4DB14968}" name="15.08.2024"/>
     <tableColumn id="178" xr3:uid="{AF270655-9049-43AD-B3E4-03050649556C}" name="20.08.2024"/>
     <tableColumn id="179" xr3:uid="{FD48276D-620C-46FF-A56F-A5DC53494BE8}" name="22.08.2024"/>
@@ -2717,8 +2717,8 @@
     <tableColumn id="210" xr3:uid="{F0008E19-D153-4DAA-B1EC-E2F000A9EF8E}" name="07.01.2025"/>
     <tableColumn id="211" xr3:uid="{D74D72D4-1406-4C66-85E6-A3BFD7541B83}" name="09.01.2025"/>
     <tableColumn id="212" xr3:uid="{FF105B19-28D8-4B89-BE28-1A7C5487EE39}" name="14.01.2025"/>
-    <tableColumn id="213" xr3:uid="{8F23ED60-899B-4518-B170-CE424D41FE6E}" name="16.01.2025" dataDxfId="2"/>
-    <tableColumn id="214" xr3:uid="{D2F3594A-D3E4-4068-A74F-46F994D484DA}" name="21.01.2025" dataDxfId="1"/>
+    <tableColumn id="213" xr3:uid="{8F23ED60-899B-4518-B170-CE424D41FE6E}" name="16.01.2025" dataDxfId="7"/>
+    <tableColumn id="214" xr3:uid="{D2F3594A-D3E4-4068-A74F-46F994D484DA}" name="21.01.2025" dataDxfId="6"/>
     <tableColumn id="215" xr3:uid="{CD40CBC8-7B23-44EC-95F5-2399A56BD388}" name="23.01.2025"/>
     <tableColumn id="216" xr3:uid="{E63CEAAB-19EF-4C33-874D-A4CCA4412E02}" name="28.01.2025"/>
     <tableColumn id="217" xr3:uid="{FF201305-BE29-4D8C-8CDD-3422A9D769A3}" name="30.01.2025"/>
@@ -2755,7 +2755,7 @@
     <tableColumn id="248" xr3:uid="{534C584C-9BEA-40ED-AD6E-D307D4B9F3EA}" name="17.06.2025"/>
     <tableColumn id="249" xr3:uid="{FE531E1F-5BCA-4EBF-AE52-75E095532D88}" name="19.06.2025"/>
     <tableColumn id="250" xr3:uid="{A5F4A3B9-ABBD-447D-B1EE-B51586C2CE25}" name="24.06.2025"/>
-    <tableColumn id="251" xr3:uid="{A9303B06-D7CF-4AEE-887B-CA2C7A50BF7C}" name="26.06.2025" dataDxfId="0"/>
+    <tableColumn id="251" xr3:uid="{A9303B06-D7CF-4AEE-887B-CA2C7A50BF7C}" name="26.06.2025" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2911,73 +2911,73 @@
     <tableColumn id="47" xr3:uid="{391F1811-EE0F-884E-8712-9715A5EC4EAF}" name="Kontrolle LLP max" dataDxfId="123">
       <calculatedColumnFormula>TBL_Grundstudium[[#This Row],[Mastery Max]]+TBL_Grundstudium[[#This Row],[ATL Max]]+TBL_Grundstudium[[#This Row],[Präsenz Max]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{93B0D6BC-5ADE-4590-A559-7B1578F3979D}" name="Note" dataDxfId="122">
-      <calculatedColumnFormula>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</calculatedColumnFormula>
+    <tableColumn id="24" xr3:uid="{93B0D6BC-5ADE-4590-A559-7B1578F3979D}" name="Note" dataDxfId="4">
+      <calculatedColumnFormula>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1C63CD85-FD5E-4C78-B083-4F597A63F5C9}" name="LLP Total" dataDxfId="121">
+    <tableColumn id="4" xr3:uid="{1C63CD85-FD5E-4C78-B083-4F597A63F5C9}" name="LLP Total" dataDxfId="122">
       <calculatedColumnFormula>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="45" xr3:uid="{4796A71A-037B-4FF9-ABA5-A414113AA179}" name="Mastery Max"/>
     <tableColumn id="22" xr3:uid="{115AED55-C979-4862-8806-EC840596709A}" name="Mastery"/>
-    <tableColumn id="44" xr3:uid="{E1AD457F-4DB6-4A7D-BF52-4143585C8C21}" name="ATL Max" dataDxfId="120"/>
-    <tableColumn id="23" xr3:uid="{5FCB314C-8652-418C-9442-962EF8547F54}" name="ATL" dataDxfId="119">
+    <tableColumn id="44" xr3:uid="{E1AD457F-4DB6-4A7D-BF52-4143585C8C21}" name="ATL Max" dataDxfId="121"/>
+    <tableColumn id="23" xr3:uid="{5FCB314C-8652-418C-9442-962EF8547F54}" name="ATL" dataDxfId="120">
       <calculatedColumnFormula>A6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{57B56113-072D-4A9B-8B69-02DDC9BDE62C}" name="Präsenz Max" dataDxfId="118">
+    <tableColumn id="43" xr3:uid="{57B56113-072D-4A9B-8B69-02DDC9BDE62C}" name="Präsenz Max" dataDxfId="119">
       <calculatedColumnFormula>VLOOKUP(TBL_Grundstudium[[#This Row],[Grundstudium]],Übersicht_Fächer!$A$2:$D$32,4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5DF7B20C-044D-46D5-9165-9BFD9A152792}" name="Präsenz" dataDxfId="117">
+    <tableColumn id="5" xr3:uid="{5DF7B20C-044D-46D5-9165-9BFD9A152792}" name="Präsenz" dataDxfId="118">
       <calculatedColumnFormula>SUM(TBL_Grundstudium[[#This Row],[01.02.2022]:[26.06.2025]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{118EA096-40EC-4749-A18D-DFD5F1604B81}" name="01.02.2022" dataDxfId="116"/>
-    <tableColumn id="7" xr3:uid="{9DB8F85E-3CA4-4D30-BAEA-0095359D48FF}" name="03.02.2022" dataDxfId="115"/>
-    <tableColumn id="8" xr3:uid="{4BD112C1-B8AE-4DF8-BA50-37AB82E46667}" name="08.02.2022" dataDxfId="114"/>
-    <tableColumn id="9" xr3:uid="{DB1CB921-2663-42B1-843B-F6517F1D8AC1}" name="10.02.2022" dataDxfId="113"/>
-    <tableColumn id="10" xr3:uid="{CBDF4C8B-3E06-4697-84B4-FF34DFB55CD5}" name="15.02.2022" dataDxfId="112"/>
-    <tableColumn id="11" xr3:uid="{B8033E1D-C14D-4C0D-909D-D77C02570E8F}" name="17.02.2022" dataDxfId="111"/>
-    <tableColumn id="12" xr3:uid="{CA1A81FC-9B8F-4B81-83CB-4251AC077B84}" name="22.02.2022" dataDxfId="110"/>
-    <tableColumn id="13" xr3:uid="{A84976CE-344E-42AA-A367-4CFD1E1A73BC}" name="24.02.2022" dataDxfId="109"/>
-    <tableColumn id="14" xr3:uid="{1610981D-76C2-4B98-9FF2-802E3860C79A}" name="15.03.2022" dataDxfId="108"/>
-    <tableColumn id="15" xr3:uid="{8597B6DA-6114-4838-9162-25943786F1EE}" name="17.03.2022" dataDxfId="107"/>
-    <tableColumn id="16" xr3:uid="{C1E70D90-09D1-4477-A1D3-4A2AC3AB91E0}" name="22.03.2022" dataDxfId="106"/>
-    <tableColumn id="17" xr3:uid="{307A4256-1BB1-443F-A7DA-E46C4B4D4415}" name="24.03.2022" dataDxfId="105"/>
-    <tableColumn id="18" xr3:uid="{5AA63F78-6245-41E1-B40D-FBDFE2029C06}" name="29.03.2022" dataDxfId="104"/>
-    <tableColumn id="19" xr3:uid="{E579F4BB-9DF6-472E-BE3F-0214ED8BC5B4}" name="31.03.2022" dataDxfId="103"/>
-    <tableColumn id="20" xr3:uid="{4B880E57-9A37-447E-AFCF-82A6BF9E6802}" name="05.04.2022" dataDxfId="102"/>
-    <tableColumn id="21" xr3:uid="{B226C903-F180-4E77-8AF7-A31025AA12BE}" name="07.04.2022" dataDxfId="101"/>
-    <tableColumn id="25" xr3:uid="{DF898180-E858-458E-8C90-1A21C36D86FA}" name="26.04.2022" dataDxfId="100"/>
-    <tableColumn id="26" xr3:uid="{021E6FF2-DF66-4425-96F3-887B68683066}" name="28.04.2022" dataDxfId="99"/>
-    <tableColumn id="27" xr3:uid="{2121E7B0-76CF-45E3-8F56-E647622D3A9B}" name="03.05.2022" dataDxfId="98"/>
-    <tableColumn id="28" xr3:uid="{B434E969-FB03-49B0-B3ED-AA5C51040D18}" name="05.05.2022" dataDxfId="97"/>
-    <tableColumn id="29" xr3:uid="{85711966-F3AB-43EE-9744-56E09C6C67BA}" name="10.05.2022" dataDxfId="96"/>
-    <tableColumn id="30" xr3:uid="{1184B567-7844-4C2A-AE83-A75489EEE85C}" name="12.05.2022" dataDxfId="95"/>
-    <tableColumn id="31" xr3:uid="{B1CA2545-23BB-40EC-97ED-B9DF80630A5A}" name="17.05.2022" dataDxfId="94"/>
-    <tableColumn id="32" xr3:uid="{C3E296E7-3B77-41A0-9E6E-EBD4325B4364}" name="19.05.2022" dataDxfId="93"/>
-    <tableColumn id="33" xr3:uid="{E81A2DD7-4F44-479D-9F6E-BB8741D81383}" name="24.05.2022" dataDxfId="92"/>
-    <tableColumn id="34" xr3:uid="{064B7898-7D90-46B0-A6F3-DF0AFD39455A}" name="31.05.2022" dataDxfId="91"/>
-    <tableColumn id="46" xr3:uid="{F071F54A-2511-474E-86B6-7B86D1AE2113}" name="02.06.2022" dataDxfId="90"/>
-    <tableColumn id="35" xr3:uid="{AB7C18CD-D23F-420C-907D-2B7327116EA2}" name="07.06.2022" dataDxfId="89"/>
-    <tableColumn id="36" xr3:uid="{70B902D8-70A9-4898-9DC7-6A6F82B4784E}" name="09.06.2022" dataDxfId="88"/>
-    <tableColumn id="37" xr3:uid="{F5D20EFA-FD84-45B2-A3AD-8EC0408B6C99}" name="14.06.2022" dataDxfId="87"/>
-    <tableColumn id="38" xr3:uid="{60830506-0AE5-4025-93D2-9DA588615E3C}" name="16.06.2022" dataDxfId="86"/>
-    <tableColumn id="39" xr3:uid="{F4C7F100-EC98-473B-87FC-6EBA68911268}" name="21.06.2022" dataDxfId="85"/>
-    <tableColumn id="40" xr3:uid="{2829DEBA-BBF1-4406-A535-105C71A56369}" name="23.06.2022" dataDxfId="84"/>
-    <tableColumn id="41" xr3:uid="{10F4FA5E-AC31-4441-9E85-B1C28E8F1971}" name="28.06.2022" dataDxfId="83"/>
-    <tableColumn id="42" xr3:uid="{1CB199F4-0C5F-4AB1-B8AF-DB037C61B6E2}" name="30.06.2022" dataDxfId="82"/>
-    <tableColumn id="48" xr3:uid="{492B54F3-E28C-42B0-963A-5AE94B56F6EA}" name="24.11.2022" dataDxfId="81"/>
-    <tableColumn id="49" xr3:uid="{1157EB07-C326-4901-803F-9D0B6D6EB783}" name="29.11.2022" dataDxfId="80"/>
-    <tableColumn id="50" xr3:uid="{F00160C4-51A2-4EBE-B894-5C929A605F48}" name="01.12.2022" dataDxfId="79"/>
-    <tableColumn id="51" xr3:uid="{5E2B07C2-5A40-4D0D-AF58-ECADA6DA7BDA}" name="06.12.2022" dataDxfId="78"/>
-    <tableColumn id="52" xr3:uid="{7D5D6C9D-C40B-4CA2-86BF-D5FDF4956AF6}" name="08.12.2022" dataDxfId="77"/>
-    <tableColumn id="53" xr3:uid="{DC819889-FED9-49A6-BB33-66B09465D361}" name="13.12.2022" dataDxfId="76"/>
-    <tableColumn id="54" xr3:uid="{FFFD7ADB-FAA7-4892-879E-ED5C3DAE1850}" name="15.12.2022" dataDxfId="75"/>
-    <tableColumn id="55" xr3:uid="{6CB9FC28-CB86-44B1-A373-9211B81C7EE2}" name="20.12.2022" dataDxfId="74"/>
-    <tableColumn id="56" xr3:uid="{73AD442E-C5BB-4C93-A606-E220958C18D6}" name="22.12.2022" dataDxfId="73"/>
-    <tableColumn id="57" xr3:uid="{425064F7-F414-4292-BB10-3342785BF8F0}" name="10.01.2023" dataDxfId="72"/>
-    <tableColumn id="58" xr3:uid="{319DFFB5-34BA-4DA0-A838-08A359AF41B9}" name="12.01.2023" dataDxfId="71"/>
-    <tableColumn id="59" xr3:uid="{FABE7E42-4B20-459C-B1DD-806F1DAB30FD}" name="17.01.2023" dataDxfId="70"/>
-    <tableColumn id="60" xr3:uid="{0F676B84-5E8F-48B8-BCF1-5CD73C006767}" name="19.01.2023" dataDxfId="69"/>
-    <tableColumn id="61" xr3:uid="{A984A99D-0DFC-4300-BBCE-24A4B5300FA5}" name="24.01.2023" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{118EA096-40EC-4749-A18D-DFD5F1604B81}" name="01.02.2022" dataDxfId="117"/>
+    <tableColumn id="7" xr3:uid="{9DB8F85E-3CA4-4D30-BAEA-0095359D48FF}" name="03.02.2022" dataDxfId="116"/>
+    <tableColumn id="8" xr3:uid="{4BD112C1-B8AE-4DF8-BA50-37AB82E46667}" name="08.02.2022" dataDxfId="115"/>
+    <tableColumn id="9" xr3:uid="{DB1CB921-2663-42B1-843B-F6517F1D8AC1}" name="10.02.2022" dataDxfId="114"/>
+    <tableColumn id="10" xr3:uid="{CBDF4C8B-3E06-4697-84B4-FF34DFB55CD5}" name="15.02.2022" dataDxfId="113"/>
+    <tableColumn id="11" xr3:uid="{B8033E1D-C14D-4C0D-909D-D77C02570E8F}" name="17.02.2022" dataDxfId="112"/>
+    <tableColumn id="12" xr3:uid="{CA1A81FC-9B8F-4B81-83CB-4251AC077B84}" name="22.02.2022" dataDxfId="111"/>
+    <tableColumn id="13" xr3:uid="{A84976CE-344E-42AA-A367-4CFD1E1A73BC}" name="24.02.2022" dataDxfId="110"/>
+    <tableColumn id="14" xr3:uid="{1610981D-76C2-4B98-9FF2-802E3860C79A}" name="15.03.2022" dataDxfId="109"/>
+    <tableColumn id="15" xr3:uid="{8597B6DA-6114-4838-9162-25943786F1EE}" name="17.03.2022" dataDxfId="108"/>
+    <tableColumn id="16" xr3:uid="{C1E70D90-09D1-4477-A1D3-4A2AC3AB91E0}" name="22.03.2022" dataDxfId="107"/>
+    <tableColumn id="17" xr3:uid="{307A4256-1BB1-443F-A7DA-E46C4B4D4415}" name="24.03.2022" dataDxfId="106"/>
+    <tableColumn id="18" xr3:uid="{5AA63F78-6245-41E1-B40D-FBDFE2029C06}" name="29.03.2022" dataDxfId="105"/>
+    <tableColumn id="19" xr3:uid="{E579F4BB-9DF6-472E-BE3F-0214ED8BC5B4}" name="31.03.2022" dataDxfId="104"/>
+    <tableColumn id="20" xr3:uid="{4B880E57-9A37-447E-AFCF-82A6BF9E6802}" name="05.04.2022" dataDxfId="103"/>
+    <tableColumn id="21" xr3:uid="{B226C903-F180-4E77-8AF7-A31025AA12BE}" name="07.04.2022" dataDxfId="102"/>
+    <tableColumn id="25" xr3:uid="{DF898180-E858-458E-8C90-1A21C36D86FA}" name="26.04.2022" dataDxfId="101"/>
+    <tableColumn id="26" xr3:uid="{021E6FF2-DF66-4425-96F3-887B68683066}" name="28.04.2022" dataDxfId="100"/>
+    <tableColumn id="27" xr3:uid="{2121E7B0-76CF-45E3-8F56-E647622D3A9B}" name="03.05.2022" dataDxfId="99"/>
+    <tableColumn id="28" xr3:uid="{B434E969-FB03-49B0-B3ED-AA5C51040D18}" name="05.05.2022" dataDxfId="98"/>
+    <tableColumn id="29" xr3:uid="{85711966-F3AB-43EE-9744-56E09C6C67BA}" name="10.05.2022" dataDxfId="97"/>
+    <tableColumn id="30" xr3:uid="{1184B567-7844-4C2A-AE83-A75489EEE85C}" name="12.05.2022" dataDxfId="96"/>
+    <tableColumn id="31" xr3:uid="{B1CA2545-23BB-40EC-97ED-B9DF80630A5A}" name="17.05.2022" dataDxfId="95"/>
+    <tableColumn id="32" xr3:uid="{C3E296E7-3B77-41A0-9E6E-EBD4325B4364}" name="19.05.2022" dataDxfId="94"/>
+    <tableColumn id="33" xr3:uid="{E81A2DD7-4F44-479D-9F6E-BB8741D81383}" name="24.05.2022" dataDxfId="93"/>
+    <tableColumn id="34" xr3:uid="{064B7898-7D90-46B0-A6F3-DF0AFD39455A}" name="31.05.2022" dataDxfId="92"/>
+    <tableColumn id="46" xr3:uid="{F071F54A-2511-474E-86B6-7B86D1AE2113}" name="02.06.2022" dataDxfId="91"/>
+    <tableColumn id="35" xr3:uid="{AB7C18CD-D23F-420C-907D-2B7327116EA2}" name="07.06.2022" dataDxfId="90"/>
+    <tableColumn id="36" xr3:uid="{70B902D8-70A9-4898-9DC7-6A6F82B4784E}" name="09.06.2022" dataDxfId="89"/>
+    <tableColumn id="37" xr3:uid="{F5D20EFA-FD84-45B2-A3AD-8EC0408B6C99}" name="14.06.2022" dataDxfId="88"/>
+    <tableColumn id="38" xr3:uid="{60830506-0AE5-4025-93D2-9DA588615E3C}" name="16.06.2022" dataDxfId="87"/>
+    <tableColumn id="39" xr3:uid="{F4C7F100-EC98-473B-87FC-6EBA68911268}" name="21.06.2022" dataDxfId="86"/>
+    <tableColumn id="40" xr3:uid="{2829DEBA-BBF1-4406-A535-105C71A56369}" name="23.06.2022" dataDxfId="85"/>
+    <tableColumn id="41" xr3:uid="{10F4FA5E-AC31-4441-9E85-B1C28E8F1971}" name="28.06.2022" dataDxfId="84"/>
+    <tableColumn id="42" xr3:uid="{1CB199F4-0C5F-4AB1-B8AF-DB037C61B6E2}" name="30.06.2022" dataDxfId="83"/>
+    <tableColumn id="48" xr3:uid="{492B54F3-E28C-42B0-963A-5AE94B56F6EA}" name="24.11.2022" dataDxfId="82"/>
+    <tableColumn id="49" xr3:uid="{1157EB07-C326-4901-803F-9D0B6D6EB783}" name="29.11.2022" dataDxfId="81"/>
+    <tableColumn id="50" xr3:uid="{F00160C4-51A2-4EBE-B894-5C929A605F48}" name="01.12.2022" dataDxfId="80"/>
+    <tableColumn id="51" xr3:uid="{5E2B07C2-5A40-4D0D-AF58-ECADA6DA7BDA}" name="06.12.2022" dataDxfId="79"/>
+    <tableColumn id="52" xr3:uid="{7D5D6C9D-C40B-4CA2-86BF-D5FDF4956AF6}" name="08.12.2022" dataDxfId="78"/>
+    <tableColumn id="53" xr3:uid="{DC819889-FED9-49A6-BB33-66B09465D361}" name="13.12.2022" dataDxfId="77"/>
+    <tableColumn id="54" xr3:uid="{FFFD7ADB-FAA7-4892-879E-ED5C3DAE1850}" name="15.12.2022" dataDxfId="76"/>
+    <tableColumn id="55" xr3:uid="{6CB9FC28-CB86-44B1-A373-9211B81C7EE2}" name="20.12.2022" dataDxfId="75"/>
+    <tableColumn id="56" xr3:uid="{73AD442E-C5BB-4C93-A606-E220958C18D6}" name="22.12.2022" dataDxfId="74"/>
+    <tableColumn id="57" xr3:uid="{425064F7-F414-4292-BB10-3342785BF8F0}" name="10.01.2023" dataDxfId="73"/>
+    <tableColumn id="58" xr3:uid="{319DFFB5-34BA-4DA0-A838-08A359AF41B9}" name="12.01.2023" dataDxfId="72"/>
+    <tableColumn id="59" xr3:uid="{FABE7E42-4B20-459C-B1DD-806F1DAB30FD}" name="17.01.2023" dataDxfId="71"/>
+    <tableColumn id="60" xr3:uid="{0F676B84-5E8F-48B8-BCF1-5CD73C006767}" name="19.01.2023" dataDxfId="70"/>
+    <tableColumn id="61" xr3:uid="{A984A99D-0DFC-4300-BBCE-24A4B5300FA5}" name="24.01.2023" dataDxfId="69"/>
     <tableColumn id="62" xr3:uid="{5FB476DA-06AE-4310-9607-88928AA6AD38}" name="26.01.2023"/>
     <tableColumn id="63" xr3:uid="{012BDC2F-17C8-48A7-AE3E-F9A10B37D486}" name="31.01.2023"/>
     <tableColumn id="64" xr3:uid="{97431CD7-F8ED-4184-9A77-A3BE860EFD58}" name="02.02.2023"/>
@@ -3014,8 +3014,8 @@
     <tableColumn id="98" xr3:uid="{CF203E54-AB2B-4AAA-9082-7D6CC6C632EC}" name="20.06.2023"/>
     <tableColumn id="99" xr3:uid="{13ECD6DE-597A-4AAC-9CCA-E9655CC74609}" name="22.06.2023"/>
     <tableColumn id="100" xr3:uid="{BB8DF66E-85C5-4C61-A9A3-826AF05F0AE6}" name="27.06.2023"/>
-    <tableColumn id="101" xr3:uid="{56F85DA1-A04A-45A9-9254-00CE808F05ED}" name="29.06.2023" dataDxfId="67"/>
-    <tableColumn id="102" xr3:uid="{B3DE2973-2568-453B-A317-09AA67C7C1DC}" name="15.08.2023" dataDxfId="66"/>
+    <tableColumn id="101" xr3:uid="{56F85DA1-A04A-45A9-9254-00CE808F05ED}" name="29.06.2023" dataDxfId="68"/>
+    <tableColumn id="102" xr3:uid="{B3DE2973-2568-453B-A317-09AA67C7C1DC}" name="15.08.2023" dataDxfId="67"/>
     <tableColumn id="70" xr3:uid="{7B2D4A7D-5050-424C-ACD9-8F16C7147AE4}" name="17.08.2023"/>
     <tableColumn id="71" xr3:uid="{D8361B91-E66E-4F2C-8A3E-C6D3E1B7D6F7}" name="22.08.2023"/>
     <tableColumn id="103" xr3:uid="{7480E393-10EC-4A7E-B4D4-B821D78BD5EC}" name="24.08.2023"/>
@@ -3052,8 +3052,8 @@
     <tableColumn id="140" xr3:uid="{F98AD6DA-4509-4F50-A830-AB384D73BCEC}" name="09.01.2024"/>
     <tableColumn id="141" xr3:uid="{DFFCEF90-7383-401D-939C-60005D5AF91B}" name="11.01.2024"/>
     <tableColumn id="142" xr3:uid="{E3219E17-B345-4953-AB2C-96DA7B5DF9E6}" name="16.01.2024"/>
-    <tableColumn id="143" xr3:uid="{A1ECB504-CA15-4F23-B632-1BECEB1A9058}" name="18.01.2024" dataDxfId="65"/>
-    <tableColumn id="144" xr3:uid="{9CCFD461-046B-4BA1-B464-13B6BE785411}" name="23.01.2024" dataDxfId="64"/>
+    <tableColumn id="143" xr3:uid="{A1ECB504-CA15-4F23-B632-1BECEB1A9058}" name="18.01.2024" dataDxfId="66"/>
+    <tableColumn id="144" xr3:uid="{9CCFD461-046B-4BA1-B464-13B6BE785411}" name="23.01.2024" dataDxfId="65"/>
     <tableColumn id="145" xr3:uid="{8DA839A1-1BB6-4D84-808A-3840F401517B}" name="25.01.2024"/>
     <tableColumn id="146" xr3:uid="{7F1E8A39-DA0B-439B-BF94-63EFF06F10E4}" name="30.01.2024"/>
     <tableColumn id="147" xr3:uid="{7A18BF0E-0B83-44BB-B3E8-385C1D159E86}" name="01.02.2024"/>
@@ -3090,8 +3090,8 @@
     <tableColumn id="186" xr3:uid="{71093CD3-0EA3-4F2B-B8CB-DED9ED5CBC4E}" name="18.06.2024"/>
     <tableColumn id="187" xr3:uid="{3F3E4810-1A7E-4A6D-A420-3E9BFA725315}" name="20.06.2024"/>
     <tableColumn id="188" xr3:uid="{0B955507-944D-4623-AEDF-C4C2856AAC6B}" name="25.06.2024"/>
-    <tableColumn id="189" xr3:uid="{320CCC08-7243-4A1A-B27C-FFC9B20D443B}" name="27.06.2024" dataDxfId="63"/>
-    <tableColumn id="202" xr3:uid="{8E2DB530-0601-4A0D-8A15-4D5F97ECF188}" name="13.08.2024" dataDxfId="62"/>
+    <tableColumn id="189" xr3:uid="{320CCC08-7243-4A1A-B27C-FFC9B20D443B}" name="27.06.2024" dataDxfId="64"/>
+    <tableColumn id="202" xr3:uid="{8E2DB530-0601-4A0D-8A15-4D5F97ECF188}" name="13.08.2024" dataDxfId="63"/>
     <tableColumn id="203" xr3:uid="{B49B718F-ED27-4E1E-AC7B-7D64DF1730A4}" name="15.08.2024"/>
     <tableColumn id="204" xr3:uid="{6B4DEB01-DE24-4BEA-8A8E-001A0C700787}" name="20.08.2024"/>
     <tableColumn id="205" xr3:uid="{2FADE9C1-A280-4F4E-8CF2-A4C10E92A278}" name="22.08.2024"/>
@@ -3128,8 +3128,8 @@
     <tableColumn id="244" xr3:uid="{9BE2483F-9D87-4F6F-9DA8-1E7DB7C23A59}" name="07.01.2025"/>
     <tableColumn id="245" xr3:uid="{A0EBF7EF-5526-4B55-9700-8864F779240B}" name="09.01.2025"/>
     <tableColumn id="246" xr3:uid="{E265CAB4-CB67-4B1A-9A75-11C8603FD36A}" name="14.01.2025"/>
-    <tableColumn id="247" xr3:uid="{737ADAE0-251D-4180-B6CD-3A06D9C54E43}" name="16.01.2025" dataDxfId="61"/>
-    <tableColumn id="248" xr3:uid="{9A9548B2-F951-43C4-BE44-3D8E2A262533}" name="21.01.2025" dataDxfId="60"/>
+    <tableColumn id="247" xr3:uid="{737ADAE0-251D-4180-B6CD-3A06D9C54E43}" name="16.01.2025" dataDxfId="62"/>
+    <tableColumn id="248" xr3:uid="{9A9548B2-F951-43C4-BE44-3D8E2A262533}" name="21.01.2025" dataDxfId="61"/>
     <tableColumn id="249" xr3:uid="{B0E3B5BD-224C-4719-9C2D-51F960E31364}" name="23.01.2025"/>
     <tableColumn id="250" xr3:uid="{13324714-8766-4C38-A6B3-95CB6C18F0C0}" name="28.01.2025"/>
     <tableColumn id="251" xr3:uid="{0190C1A8-1EAF-4863-B636-583C6F9F6929}" name="30.01.2025"/>
@@ -3166,7 +3166,7 @@
     <tableColumn id="290" xr3:uid="{AF0E05D1-1144-4307-9971-80A4688DE121}" name="17.06.2025"/>
     <tableColumn id="291" xr3:uid="{FC47CCC8-243E-4752-830D-2107BCF9D63C}" name="19.06.2025"/>
     <tableColumn id="292" xr3:uid="{29778C20-805C-436C-AEBF-6D59F95C47BF}" name="24.06.2025"/>
-    <tableColumn id="293" xr3:uid="{0A1432B0-22F4-48B1-9630-E324E66B4112}" name="26.06.2025" dataDxfId="59"/>
+    <tableColumn id="293" xr3:uid="{0A1432B0-22F4-48B1-9630-E324E66B4112}" name="26.06.2025" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3178,30 +3178,30 @@
   <tableColumns count="251">
     <tableColumn id="1" xr3:uid="{AEB1C7EE-9393-4DCE-9662-FE6024C78634}" name="Kommunikation &amp; Führung"/>
     <tableColumn id="2" xr3:uid="{C16E187D-5757-4893-BC3D-E992159BC68B}" name="Fach"/>
-    <tableColumn id="67" xr3:uid="{1A93E11A-643E-435A-A358-2D693E7CC530}" name="Status" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{94DB570D-D8A9-437B-A224-3DFED36FEE0A}" name="LLP max" dataDxfId="57">
+    <tableColumn id="67" xr3:uid="{1A93E11A-643E-435A-A358-2D693E7CC530}" name="Status" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{94DB570D-D8A9-437B-A224-3DFED36FEE0A}" name="LLP max" dataDxfId="58">
       <calculatedColumnFormula>VLOOKUP(TBL_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],Übersicht_Fächer!$A$2:$E$32,5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{D29F72AB-6E7B-0342-8351-6FF804E68D8B}" name="Kontrolle LLP max" dataDxfId="56">
+    <tableColumn id="47" xr3:uid="{D29F72AB-6E7B-0342-8351-6FF804E68D8B}" name="Kontrolle LLP max" dataDxfId="57">
       <calculatedColumnFormula>TBL_Kommunikation[[#This Row],[Mastery Max]]+TBL_Kommunikation[[#This Row],[ATL Max]]+TBL_Kommunikation[[#This Row],[Präsenz Max]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{C8A9F2E1-E1C8-4CBE-B012-DB7D53BCC34B}" name="Note" dataDxfId="55">
-      <calculatedColumnFormula>IF(((TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5))</calculatedColumnFormula>
+    <tableColumn id="24" xr3:uid="{C8A9F2E1-E1C8-4CBE-B012-DB7D53BCC34B}" name="Note" dataDxfId="3">
+      <calculatedColumnFormula>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DEDF4D39-AB24-42BF-961A-2386150F6639}" name="LLP Total" dataDxfId="54">
+    <tableColumn id="4" xr3:uid="{DEDF4D39-AB24-42BF-961A-2386150F6639}" name="LLP Total" dataDxfId="56">
       <calculatedColumnFormula>TBL_Kommunikation[[#This Row],[Mastery]]+TBL_Kommunikation[[#This Row],[ATL]]+TBL_Kommunikation[[#This Row],[Präsenz]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="45" xr3:uid="{49CA61D9-69BD-46C8-AA94-2AF9D7148CB0}" name="Mastery Max"/>
     <tableColumn id="23" xr3:uid="{50A0650C-C40A-4837-B6CF-E4434A1C3464}" name="Mastery"/>
     <tableColumn id="44" xr3:uid="{DE6E4043-1B0E-419B-B802-E4B583DC1F0C}" name="ATL Max"/>
     <tableColumn id="22" xr3:uid="{F4B26F9F-D729-43B2-8D81-FC926BEFC46D}" name="ATL"/>
-    <tableColumn id="43" xr3:uid="{020BB2F6-84BE-4C73-945D-A7A29B22B7F8}" name="Präsenz Max" dataDxfId="53">
+    <tableColumn id="43" xr3:uid="{020BB2F6-84BE-4C73-945D-A7A29B22B7F8}" name="Präsenz Max" dataDxfId="55">
       <calculatedColumnFormula>VLOOKUP(TBL_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],Übersicht_Fächer!$A$2:$D$32,4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BEA6583E-4356-433D-B2FE-FE5EE2E02D49}" name="Präsenz" dataDxfId="52">
+    <tableColumn id="5" xr3:uid="{BEA6583E-4356-433D-B2FE-FE5EE2E02D49}" name="Präsenz" dataDxfId="54">
       <calculatedColumnFormula>SUM(TBL_Kommunikation[[#This Row],[01.02.2022]:[26.06.2025]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{634BDB4A-6E2F-49B8-8D12-C7C15F922BCE}" name="01.02.2022" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{634BDB4A-6E2F-49B8-8D12-C7C15F922BCE}" name="01.02.2022" dataDxfId="53"/>
     <tableColumn id="7" xr3:uid="{D6EF1FC8-1260-4D71-BE2C-0C6FCA74643D}" name="03.02.2022"/>
     <tableColumn id="8" xr3:uid="{782C1F7E-5123-4757-85A5-3F65883F6A98}" name="08.02.2022"/>
     <tableColumn id="9" xr3:uid="{8904746C-214C-4349-887D-3D50119A9A4A}" name="10.02.2022"/>
@@ -3248,8 +3248,8 @@
     <tableColumn id="57" xr3:uid="{29E6C366-A733-485F-927C-34244B652026}" name="10.01.2023"/>
     <tableColumn id="58" xr3:uid="{25F7468F-72FB-4AD9-92B9-3F2CEA6077AE}" name="12.01.2023"/>
     <tableColumn id="59" xr3:uid="{AE0C0B8F-1B0F-4F52-94DE-EEAD936C3DEB}" name="17.01.2023"/>
-    <tableColumn id="60" xr3:uid="{BBD85A0F-525F-412D-B6CB-E2524EF2F85E}" name="19.01.2023" dataDxfId="50"/>
-    <tableColumn id="61" xr3:uid="{8515C8C2-A082-486E-812F-32E51E99F4C0}" name="24.01.2023" dataDxfId="49"/>
+    <tableColumn id="60" xr3:uid="{BBD85A0F-525F-412D-B6CB-E2524EF2F85E}" name="19.01.2023" dataDxfId="52"/>
+    <tableColumn id="61" xr3:uid="{8515C8C2-A082-486E-812F-32E51E99F4C0}" name="24.01.2023" dataDxfId="51"/>
     <tableColumn id="62" xr3:uid="{396697AB-3A4C-4D0E-9D8B-7096FD128403}" name="26.01.2023"/>
     <tableColumn id="63" xr3:uid="{66B581FE-21B9-4306-B62A-C656C0871912}" name="31.01.2023"/>
     <tableColumn id="64" xr3:uid="{7A187CB2-2AA2-4E43-8004-C454046BF9BA}" name="02.02.2023"/>
@@ -3286,8 +3286,8 @@
     <tableColumn id="96" xr3:uid="{4B5211AC-1B4B-44A0-955A-234AA97459B3}" name="20.06.2023"/>
     <tableColumn id="97" xr3:uid="{6E07E536-01F3-4083-BF2C-9488B94B9B08}" name="22.06.2023"/>
     <tableColumn id="98" xr3:uid="{922ED6D7-DD36-424B-B11D-9BF1673C5EE4}" name="27.06.2023"/>
-    <tableColumn id="99" xr3:uid="{043B38E0-4ACD-4EC2-B87A-B1B164763518}" name="29.06.2023" dataDxfId="48"/>
-    <tableColumn id="100" xr3:uid="{01900FC2-F523-465E-9FA4-53BE9BE2A676}" name="15.08.2023" dataDxfId="47"/>
+    <tableColumn id="99" xr3:uid="{043B38E0-4ACD-4EC2-B87A-B1B164763518}" name="29.06.2023" dataDxfId="50"/>
+    <tableColumn id="100" xr3:uid="{01900FC2-F523-465E-9FA4-53BE9BE2A676}" name="15.08.2023" dataDxfId="49"/>
     <tableColumn id="101" xr3:uid="{3EC42AE1-B127-4E79-B97E-59D5B446F23A}" name="17.08.2023"/>
     <tableColumn id="102" xr3:uid="{333FF37A-16B2-4EF1-AC70-0FDF4BB14B1F}" name="22.08.2023"/>
     <tableColumn id="103" xr3:uid="{EA252331-B7E2-4012-857C-5730062A75EA}" name="24.08.2023"/>
@@ -3324,8 +3324,8 @@
     <tableColumn id="134" xr3:uid="{3E702944-99EC-4788-839D-52E8F30970AF}" name="09.01.2024"/>
     <tableColumn id="135" xr3:uid="{8FB3F35A-E772-40C3-B363-618BDBB0D5F5}" name="11.01.2024"/>
     <tableColumn id="136" xr3:uid="{ACB3A6E5-28C3-4602-A9CC-B44CA43A3F71}" name="16.01.2024"/>
-    <tableColumn id="137" xr3:uid="{962B14B0-FEBF-4FFC-9BC7-2CDA67C520FF}" name="18.01.2024" dataDxfId="46"/>
-    <tableColumn id="138" xr3:uid="{40BEFE29-6825-4006-B309-79FC3CA29501}" name="23.01.2024" dataDxfId="45"/>
+    <tableColumn id="137" xr3:uid="{962B14B0-FEBF-4FFC-9BC7-2CDA67C520FF}" name="18.01.2024" dataDxfId="48"/>
+    <tableColumn id="138" xr3:uid="{40BEFE29-6825-4006-B309-79FC3CA29501}" name="23.01.2024" dataDxfId="47"/>
     <tableColumn id="139" xr3:uid="{77287EC5-CA63-4A9A-8DFA-81610DD0BBE3}" name="25.01.2024"/>
     <tableColumn id="140" xr3:uid="{015E3D6C-17B5-421D-817B-FE1865434971}" name="30.01.2024"/>
     <tableColumn id="141" xr3:uid="{316C3343-5F6A-4062-94E9-09CC547480C7}" name="01.02.2024"/>
@@ -3362,8 +3362,8 @@
     <tableColumn id="172" xr3:uid="{74755FF5-AA73-4627-B2E0-D0BB5A306F0D}" name="18.06.2024"/>
     <tableColumn id="173" xr3:uid="{3F853BCB-FA3C-4C40-AA50-38D4F0EE1387}" name="20.06.2024"/>
     <tableColumn id="174" xr3:uid="{7C396039-E613-4EAA-80A6-C521D1156460}" name="25.06.2024"/>
-    <tableColumn id="175" xr3:uid="{33EC2CAF-E3FB-4459-86F7-EFB673A824CF}" name="27.06.2024" dataDxfId="44"/>
-    <tableColumn id="176" xr3:uid="{89327000-3258-496B-AC14-D97BC1B526F6}" name="13.08.2024" dataDxfId="43"/>
+    <tableColumn id="175" xr3:uid="{33EC2CAF-E3FB-4459-86F7-EFB673A824CF}" name="27.06.2024" dataDxfId="46"/>
+    <tableColumn id="176" xr3:uid="{89327000-3258-496B-AC14-D97BC1B526F6}" name="13.08.2024" dataDxfId="45"/>
     <tableColumn id="177" xr3:uid="{D2A5B056-83D5-4A0D-9754-18A4C757FAB7}" name="15.08.2024"/>
     <tableColumn id="178" xr3:uid="{6669F6C2-F483-4B7C-A8F2-EB4E2F522EDC}" name="20.08.2024"/>
     <tableColumn id="179" xr3:uid="{25AC6CBD-1916-44BA-A55D-F309E6A5A115}" name="22.08.2024"/>
@@ -3400,8 +3400,8 @@
     <tableColumn id="210" xr3:uid="{12C71186-BC3D-400F-9279-3589F6D81E19}" name="07.01.2025"/>
     <tableColumn id="211" xr3:uid="{21A84BD4-8F90-47AD-9EA6-5E76DF53D652}" name="09.01.2025"/>
     <tableColumn id="212" xr3:uid="{F4F60777-82EC-48EB-999F-693B1291CF31}" name="14.01.2025"/>
-    <tableColumn id="213" xr3:uid="{AF587AB0-9132-476A-B7F2-E9228855F5C5}" name="16.01.2025" dataDxfId="42"/>
-    <tableColumn id="214" xr3:uid="{94AB1AA9-E8ED-4EFE-B350-5F069F28412F}" name="21.01.2025" dataDxfId="41"/>
+    <tableColumn id="213" xr3:uid="{AF587AB0-9132-476A-B7F2-E9228855F5C5}" name="16.01.2025" dataDxfId="44"/>
+    <tableColumn id="214" xr3:uid="{94AB1AA9-E8ED-4EFE-B350-5F069F28412F}" name="21.01.2025" dataDxfId="43"/>
     <tableColumn id="215" xr3:uid="{E5E98B60-79D2-4206-AFB8-875DF9E9543A}" name="23.01.2025"/>
     <tableColumn id="216" xr3:uid="{2806E830-DA1A-4961-BD03-5C0C5A6008D1}" name="28.01.2025"/>
     <tableColumn id="217" xr3:uid="{C1F51611-8BF2-436F-BB12-6A44710C9384}" name="30.01.2025"/>
@@ -3438,7 +3438,7 @@
     <tableColumn id="248" xr3:uid="{4B41CD92-5955-454A-843E-FA85CFFF31D8}" name="17.06.2025"/>
     <tableColumn id="249" xr3:uid="{00C63C65-61FE-4C4D-A71F-E94B7FF5DE39}" name="19.06.2025"/>
     <tableColumn id="250" xr3:uid="{F2612EC7-B610-45E6-A3B7-E325AC244230}" name="24.06.2025"/>
-    <tableColumn id="251" xr3:uid="{B697737A-5377-41A7-BB34-5A5DBD631BF0}" name="26.06.2025" dataDxfId="40"/>
+    <tableColumn id="251" xr3:uid="{B697737A-5377-41A7-BB34-5A5DBD631BF0}" name="26.06.2025" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3450,30 +3450,30 @@
   <tableColumns count="251">
     <tableColumn id="1" xr3:uid="{0C5015E0-08BA-48E2-9F7F-736A1B3102DA}" name="Schwerpunkt Systemtechnik"/>
     <tableColumn id="2" xr3:uid="{31916DC7-3025-411E-B8AB-CD4963424EAB}" name="Fach"/>
-    <tableColumn id="67" xr3:uid="{4E1449EB-E0ED-4182-90E5-DD575BCEE7C0}" name="Status" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{B69D1F1D-3F2B-4A98-B688-94E84AA1F186}" name="LLP max" dataDxfId="38">
+    <tableColumn id="67" xr3:uid="{4E1449EB-E0ED-4182-90E5-DD575BCEE7C0}" name="Status" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{B69D1F1D-3F2B-4A98-B688-94E84AA1F186}" name="LLP max" dataDxfId="40">
       <calculatedColumnFormula>VLOOKUP(TBL_S_System[[#This Row],[Schwerpunkt Systemtechnik]],Übersicht_Fächer!$A$2:$E$32,5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{8602DB17-0FFF-064B-BF28-A8B42C458D70}" name="Kontrolle LLP max" dataDxfId="37">
+    <tableColumn id="47" xr3:uid="{8602DB17-0FFF-064B-BF28-A8B42C458D70}" name="Kontrolle LLP max" dataDxfId="39">
       <calculatedColumnFormula>TBL_S_System[[#This Row],[Mastery Max]]+TBL_S_System[[#This Row],[ATL Max]]+TBL_S_System[[#This Row],[Präsenz Max]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{ECF2CE53-2E14-4BFB-9B0F-74C1B43C8821}" name="Note" dataDxfId="36">
-      <calculatedColumnFormula>IF(((TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5))</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{ECF2CE53-2E14-4BFB-9B0F-74C1B43C8821}" name="Note" dataDxfId="2">
+      <calculatedColumnFormula>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{54181AB0-5314-4A6D-A364-D83146CB91F9}" name="LLP Total" dataDxfId="35">
+    <tableColumn id="23" xr3:uid="{54181AB0-5314-4A6D-A364-D83146CB91F9}" name="LLP Total" dataDxfId="38">
       <calculatedColumnFormula>TBL_S_System[[#This Row],[Mastery]]+TBL_S_System[[#This Row],[ATL]]+TBL_S_System[[#This Row],[Präsenz]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="45" xr3:uid="{37BADAAF-9EBC-40C7-A0B4-BDDB45854846}" name="Mastery Max"/>
     <tableColumn id="22" xr3:uid="{0CCF1C43-D66C-41C9-B3CA-11FE6904B27C}" name="Mastery"/>
     <tableColumn id="44" xr3:uid="{6922F1C1-41C6-43CF-9B0D-17920D54A958}" name="ATL Max"/>
     <tableColumn id="24" xr3:uid="{F5392DEF-7F98-43A8-8BDC-566158108D44}" name="ATL"/>
-    <tableColumn id="43" xr3:uid="{6B5AC86D-6A7A-4F3C-B401-51CF4899C78C}" name="Präsenz Max" dataDxfId="34">
+    <tableColumn id="43" xr3:uid="{6B5AC86D-6A7A-4F3C-B401-51CF4899C78C}" name="Präsenz Max" dataDxfId="37">
       <calculatedColumnFormula>VLOOKUP(TBL_S_System[[#This Row],[Schwerpunkt Systemtechnik]],Übersicht_Fächer!$A$2:$D$32,4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{DBD3C8FD-394B-4CAF-BFA9-FADD6A27B431}" name="Präsenz" dataDxfId="33">
+    <tableColumn id="5" xr3:uid="{DBD3C8FD-394B-4CAF-BFA9-FADD6A27B431}" name="Präsenz" dataDxfId="36">
       <calculatedColumnFormula>SUM(TBL_S_System[[#This Row],[01.02.2022]:[26.06.2025]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3971D41D-AF8D-4CE2-B451-9804386E9F2F}" name="01.02.2022" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{3971D41D-AF8D-4CE2-B451-9804386E9F2F}" name="01.02.2022" dataDxfId="35"/>
     <tableColumn id="7" xr3:uid="{ADFB47AE-1F5E-4AA6-9BAC-3CCB64A52A1A}" name="03.02.2022"/>
     <tableColumn id="8" xr3:uid="{92075445-9C62-477E-8AA3-C18039C29C0C}" name="08.02.2022"/>
     <tableColumn id="9" xr3:uid="{C5C9D01E-A2A2-4AE1-BD9A-7DB501016213}" name="10.02.2022"/>
@@ -3520,8 +3520,8 @@
     <tableColumn id="57" xr3:uid="{FE7EB227-ECFB-4463-BA7A-6BB3804F3824}" name="10.01.2023"/>
     <tableColumn id="58" xr3:uid="{56CF28B7-5959-4232-BA3B-8A8963195C74}" name="12.01.2023"/>
     <tableColumn id="59" xr3:uid="{E4BE00E0-FE31-46E0-A83A-22C710C2D2DC}" name="17.01.2023"/>
-    <tableColumn id="60" xr3:uid="{AB75361B-60A5-4BAA-91F7-2F3E4C552E46}" name="19.01.2023" dataDxfId="31"/>
-    <tableColumn id="61" xr3:uid="{D59E21D6-8715-4C52-BBE3-1A0455084D4E}" name="24.01.2023" dataDxfId="30"/>
+    <tableColumn id="60" xr3:uid="{AB75361B-60A5-4BAA-91F7-2F3E4C552E46}" name="19.01.2023" dataDxfId="34"/>
+    <tableColumn id="61" xr3:uid="{D59E21D6-8715-4C52-BBE3-1A0455084D4E}" name="24.01.2023" dataDxfId="33"/>
     <tableColumn id="62" xr3:uid="{CA097E5D-825D-4B8D-B242-9DFE1166D9A5}" name="26.01.2023"/>
     <tableColumn id="63" xr3:uid="{64BA73B2-80F4-496C-A7E2-76F93B397994}" name="31.01.2023"/>
     <tableColumn id="64" xr3:uid="{02408FE0-CFB0-49D6-9B28-B7183DA1CB28}" name="02.02.2023"/>
@@ -3558,8 +3558,8 @@
     <tableColumn id="96" xr3:uid="{13DAC057-11FF-4609-8A32-04B2ADE8EE62}" name="20.06.2023"/>
     <tableColumn id="97" xr3:uid="{6D48F509-B30A-4B54-A7BC-B0739DA41AC4}" name="22.06.2023"/>
     <tableColumn id="98" xr3:uid="{06BF5951-6895-472C-AB62-D4DFB87FE21F}" name="27.06.2023"/>
-    <tableColumn id="99" xr3:uid="{EC52FBA0-5796-4842-AF48-6AC1C91D733B}" name="29.06.2023" dataDxfId="29"/>
-    <tableColumn id="100" xr3:uid="{E34E4266-B5C1-4720-B6B3-B5440DC271EB}" name="15.08.2023" dataDxfId="28"/>
+    <tableColumn id="99" xr3:uid="{EC52FBA0-5796-4842-AF48-6AC1C91D733B}" name="29.06.2023" dataDxfId="32"/>
+    <tableColumn id="100" xr3:uid="{E34E4266-B5C1-4720-B6B3-B5440DC271EB}" name="15.08.2023" dataDxfId="31"/>
     <tableColumn id="101" xr3:uid="{05C67583-F09D-4552-B65A-CC32413F550A}" name="17.08.2023"/>
     <tableColumn id="102" xr3:uid="{69AA440C-9AE6-4C34-800F-FBEA2BBFD29D}" name="22.08.2023"/>
     <tableColumn id="103" xr3:uid="{4A1B5CE0-E5CC-4C14-A4DC-508B6DA953B0}" name="24.08.2023"/>
@@ -3596,8 +3596,8 @@
     <tableColumn id="134" xr3:uid="{8B4A9914-2D08-4212-8EE3-B12636F089A1}" name="09.01.2024"/>
     <tableColumn id="135" xr3:uid="{447F037D-4E54-4EA1-ADDF-22DDEBAFA2D4}" name="11.01.2024"/>
     <tableColumn id="136" xr3:uid="{1DB57EAD-E976-4DB3-A536-73199C79AEAA}" name="16.01.2024"/>
-    <tableColumn id="137" xr3:uid="{F83A14D7-F4D1-4196-B6A9-C2FFD8D94188}" name="18.01.2024" dataDxfId="27"/>
-    <tableColumn id="138" xr3:uid="{F9CB5C53-4348-4972-BE11-0380D585441E}" name="23.01.2024" dataDxfId="26"/>
+    <tableColumn id="137" xr3:uid="{F83A14D7-F4D1-4196-B6A9-C2FFD8D94188}" name="18.01.2024" dataDxfId="30"/>
+    <tableColumn id="138" xr3:uid="{F9CB5C53-4348-4972-BE11-0380D585441E}" name="23.01.2024" dataDxfId="29"/>
     <tableColumn id="139" xr3:uid="{70F742DF-B571-4815-9B24-4367B4B16167}" name="25.01.2024"/>
     <tableColumn id="140" xr3:uid="{A5B15207-4611-4618-9D33-EDB6F327F3C7}" name="30.01.2024"/>
     <tableColumn id="141" xr3:uid="{D7B7675B-A9BF-4D13-9A57-0C5045E21909}" name="01.02.2024"/>
@@ -3634,8 +3634,8 @@
     <tableColumn id="172" xr3:uid="{D3E3B9D0-9531-441C-B789-8B95EC1D5D1F}" name="18.06.2024"/>
     <tableColumn id="173" xr3:uid="{7599230C-1E7B-471D-B2F3-ADD32796AFED}" name="20.06.2024"/>
     <tableColumn id="174" xr3:uid="{47235ADD-54AC-4C6F-B2FC-12D8C3365DA2}" name="25.06.2024"/>
-    <tableColumn id="175" xr3:uid="{2D1306F7-F20C-4BBF-8883-F9F634FF652A}" name="27.06.2024" dataDxfId="25"/>
-    <tableColumn id="176" xr3:uid="{2B60B4FE-77E7-408B-B6D1-F3B6C22E228D}" name="13.08.2024" dataDxfId="24"/>
+    <tableColumn id="175" xr3:uid="{2D1306F7-F20C-4BBF-8883-F9F634FF652A}" name="27.06.2024" dataDxfId="28"/>
+    <tableColumn id="176" xr3:uid="{2B60B4FE-77E7-408B-B6D1-F3B6C22E228D}" name="13.08.2024" dataDxfId="27"/>
     <tableColumn id="177" xr3:uid="{04AD8E41-6FAD-4EC2-AC34-6AC049A6AE28}" name="15.08.2024"/>
     <tableColumn id="178" xr3:uid="{E55B0E9F-F236-45FE-9820-E252277431D6}" name="20.08.2024"/>
     <tableColumn id="179" xr3:uid="{E2759FF8-BE24-4888-BF01-F2D768DC0D75}" name="22.08.2024"/>
@@ -3672,8 +3672,8 @@
     <tableColumn id="210" xr3:uid="{F5B368A0-0717-4893-A834-00CA79B46A4B}" name="07.01.2025"/>
     <tableColumn id="211" xr3:uid="{2A26CFD5-72FE-4073-8F57-485B3DEE220E}" name="09.01.2025"/>
     <tableColumn id="212" xr3:uid="{801FD813-181B-4151-9802-6D518F913C82}" name="14.01.2025"/>
-    <tableColumn id="213" xr3:uid="{3594DAD5-3E67-41D1-AE6B-5C42B6F58CAA}" name="16.01.2025" dataDxfId="23"/>
-    <tableColumn id="214" xr3:uid="{FCB68AAE-1A2C-4FB5-AD02-5F04FA6672FE}" name="21.01.2025" dataDxfId="22"/>
+    <tableColumn id="213" xr3:uid="{3594DAD5-3E67-41D1-AE6B-5C42B6F58CAA}" name="16.01.2025" dataDxfId="26"/>
+    <tableColumn id="214" xr3:uid="{FCB68AAE-1A2C-4FB5-AD02-5F04FA6672FE}" name="21.01.2025" dataDxfId="25"/>
     <tableColumn id="215" xr3:uid="{6A60BB04-6A53-45C0-82D6-42F5E0B3F347}" name="23.01.2025"/>
     <tableColumn id="216" xr3:uid="{E63CD5C7-C77B-40B6-AB75-8842CBC914DD}" name="28.01.2025"/>
     <tableColumn id="217" xr3:uid="{AA5D73CC-8929-4E5D-A37D-47C6AC77E542}" name="30.01.2025"/>
@@ -3710,7 +3710,7 @@
     <tableColumn id="248" xr3:uid="{EE896401-1954-4435-9777-46881B9C7514}" name="17.06.2025"/>
     <tableColumn id="249" xr3:uid="{4A824428-B19A-403C-B00B-0656FC532685}" name="19.06.2025"/>
     <tableColumn id="250" xr3:uid="{C41D1C95-21CA-47EB-8B9C-307B71CF430C}" name="24.06.2025"/>
-    <tableColumn id="251" xr3:uid="{7F91390F-518E-4F0E-9D78-A597B8AB0503}" name="26.06.2025" dataDxfId="21"/>
+    <tableColumn id="251" xr3:uid="{7F91390F-518E-4F0E-9D78-A597B8AB0503}" name="26.06.2025" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4017,26 +4017,26 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -4065,11 +4065,11 @@
         <v>1368</v>
       </c>
       <c r="E4">
-        <f>IFERROR(IF(((SUM(TBL_Ü_Grund[LLP total])/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(SUM(TBL_Ü_Grund[LLP total])/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <f>IF(SUM(TBL_Ü_Grund[LLP total])&gt;=SUM(TBL_Ü_Grund[LLP max])*0.9,6,IF(SUM(TBL_Ü_Grund[LLP total])&lt;=SUM(TBL_Ü_Grund[LLP max])*0.16,1,IF(SUM(TBL_Ü_Grund[LLP total])&gt;SUM(TBL_Ü_Grund[LLP max])*0.6,(2/((SUM(TBL_Ü_Grund[LLP max])*0.9)-(SUM(TBL_Ü_Grund[LLP max])*0.6))*SUM(TBL_Ü_Grund[LLP total])),(4/((SUM(TBL_Ü_Grund[LLP max])*0.6)-SUM(TBL_Ü_Grund[LLP max])*0.16))*SUM(TBL_Ü_Grund[LLP total]))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>32</v>
       </c>
@@ -4081,11 +4081,11 @@
         <v>576</v>
       </c>
       <c r="E5">
-        <f>IFERROR(IF(((SUM(TBL_Ü_Kommunikation[LLP total])/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(SUM(TBL_Ü_Kommunikation[LLP total])/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <f>IF(SUM(TBL_Ü_Kommunikation[LLP total])&gt;=SUM(TBL_Ü_Kommunikation[LLP max])*0.9,6,IF(SUM(TBL_Ü_Kommunikation[LLP total])&lt;=SUM(TBL_Ü_Kommunikation[LLP max])*0.16,1,IF(SUM(TBL_Ü_Kommunikation[LLP total])&gt;SUM(TBL_Ü_Kommunikation[LLP max])*0.6,(2/((SUM(TBL_Ü_Kommunikation[LLP max])*0.9)-(SUM(TBL_Ü_Kommunikation[LLP max])*0.6))*SUM(TBL_Ü_Kommunikation[LLP total])),(4/((SUM(TBL_Ü_Kommunikation[LLP max])*0.6)-SUM(TBL_Ü_Kommunikation[LLP max])*0.16))*SUM(TBL_Ü_Kommunikation[LLP total]))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>45</v>
       </c>
@@ -4097,11 +4097,11 @@
         <v>864</v>
       </c>
       <c r="E6">
-        <f>IFERROR(IF(((SUM(TBL_Ü_S_System[LLP total])/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(SUM(TBL_Ü_S_System[LLP total])/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <f>IF(SUM(TBL_Ü_S_System[LLP total])&gt;=SUM(TBL_Ü_S_System[LLP max])*0.9,6,IF(SUM(TBL_Ü_S_System[LLP total])&lt;=SUM(TBL_Ü_S_System[LLP max])*0.16,1,IF(SUM(TBL_Ü_S_System[LLP total])&gt;SUM(TBL_Ü_S_System[LLP max])*0.6,(2/((SUM(TBL_Ü_S_System[LLP max])*0.9)-(SUM(TBL_Ü_S_System[LLP max])*0.6))*SUM(TBL_Ü_S_System[LLP total])),(4/((SUM(TBL_Ü_S_System[LLP max])*0.6)-SUM(TBL_Ü_S_System[LLP max])*0.16))*SUM(TBL_Ü_S_System[LLP total]))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>153</v>
       </c>
@@ -4113,11 +4113,11 @@
         <v>864</v>
       </c>
       <c r="E7">
-        <f>IFERROR(IF(((SUM(TBL_Ü_S_Software[LLP total])/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(SUM(TBL_Ü_S_Software[LLP total])/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <f>IF(SUM(TBL_Ü_S_Software[LLP total])&gt;=SUM(TBL_Ü_S_Software[LLP max])*0.9,6,IF(SUM(TBL_Ü_S_Software[LLP total])&lt;=SUM(TBL_Ü_S_Software[LLP max])*0.16,1,IF(SUM(TBL_Ü_S_Software[LLP total])&gt;SUM(TBL_Ü_S_Software[LLP max])*0.6,(2/((SUM(TBL_Ü_S_Software[LLP max])*0.9)-(SUM(TBL_Ü_S_Software[LLP max])*0.6))*SUM(TBL_Ü_S_Software[LLP total])),(4/((SUM(TBL_Ü_S_Software[LLP max])*0.6)-SUM(TBL_Ü_S_Software[LLP max])*0.16))*SUM(TBL_Ü_S_Software[LLP total]))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>114</v>
       </c>
@@ -4129,11 +4129,11 @@
         <v>400</v>
       </c>
       <c r="E8">
-        <f>IFERROR(IF(((SUM(F59)/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(SUM(F59)/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <f>E59</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>121</v>
       </c>
@@ -4145,11 +4145,11 @@
         <v>72</v>
       </c>
       <c r="E9">
-        <f>IFERROR(IF(((SUM(F60)/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(SUM(F60)/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <f>E60</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>120</v>
       </c>
@@ -4161,11 +4161,11 @@
         <v>600</v>
       </c>
       <c r="E10">
-        <f>IFERROR(IF(((SUM(F61)/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(SUM(F61)/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <f>E61</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>105</v>
       </c>
@@ -4177,11 +4177,11 @@
         <v>120</v>
       </c>
       <c r="E11">
-        <f>IFERROR(IF(((SUM(F62)/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(SUM(F62)/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <f>E62</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>181</v>
       </c>
@@ -4195,12 +4195,9 @@
         <f>SUM(D4:D6,D8:D11)</f>
         <v>4000</v>
       </c>
-      <c r="E12" s="5">
-        <f>IFERROR(IF(((SUM(TBL_Ü_Grund[LLP total],TBL_Ü_Kommunikation[LLP total],TBL_Ü_S_System[LLP total],TBL_Ü_S_Software[LLP total],TBL_Ü_Allgemein[Total LLP])/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(SUM(TBL_Ü_Grund[LLP total],TBL_Ü_Kommunikation[LLP total],TBL_Ü_S_System[LLP total],TBL_Ü_S_Software[LLP total],TBL_Ü_Allgemein[Total LLP])/(TBL_Gesamt[[#This Row],[LLP max]]*0.9)*5)),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -4229,7 +4226,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -4246,7 +4243,7 @@
       </c>
       <c r="E15" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4265,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -4282,7 +4279,7 @@
       </c>
       <c r="E16" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4301,7 +4298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -4318,7 +4315,7 @@
       </c>
       <c r="E17" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4337,7 +4334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -4354,7 +4351,7 @@
       </c>
       <c r="E18" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4373,7 +4370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -4390,7 +4387,7 @@
       </c>
       <c r="E19" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4409,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -4426,7 +4423,7 @@
       </c>
       <c r="E20" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4445,7 +4442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -4462,7 +4459,7 @@
       </c>
       <c r="E21" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4481,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -4498,7 +4495,7 @@
       </c>
       <c r="E22" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4517,7 +4514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -4534,7 +4531,7 @@
       </c>
       <c r="E23" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4553,7 +4550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -4570,7 +4567,7 @@
       </c>
       <c r="E24" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4589,7 +4586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -4606,7 +4603,7 @@
       </c>
       <c r="E25" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4625,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -4642,7 +4639,7 @@
       </c>
       <c r="E26" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4661,7 +4658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -4678,7 +4675,7 @@
       </c>
       <c r="E27" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="9">
         <f>VLOOKUP(TBL_Ü_Grund[[#This Row],[Grundstudium]],TBL_Grundstudium[#All],7,FALSE)</f>
@@ -4697,7 +4694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -4726,7 +4723,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -4743,7 +4740,7 @@
       </c>
       <c r="E30" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],7,FALSE)</f>
@@ -4762,7 +4759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -4779,7 +4776,7 @@
       </c>
       <c r="E31" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],7,FALSE)</f>
@@ -4798,7 +4795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -4815,7 +4812,7 @@
       </c>
       <c r="E32" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],7,FALSE)</f>
@@ -4834,7 +4831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -4851,7 +4848,7 @@
       </c>
       <c r="E33" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],7,FALSE)</f>
@@ -4870,7 +4867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -4887,7 +4884,7 @@
       </c>
       <c r="E34" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],7,FALSE)</f>
@@ -4906,7 +4903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -4923,7 +4920,7 @@
       </c>
       <c r="E35" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="9">
         <f>VLOOKUP(TBL_Ü_Kommunikation[[#This Row],[Kommunikation &amp; Führung]],TBL_Kommunikation[#All],7,FALSE)</f>
@@ -4942,7 +4939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -4971,7 +4968,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -4988,7 +4985,7 @@
       </c>
       <c r="E38" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],7,FALSE)</f>
@@ -5007,7 +5004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -5024,7 +5021,7 @@
       </c>
       <c r="E39" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],7,FALSE)</f>
@@ -5043,7 +5040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -5060,7 +5057,7 @@
       </c>
       <c r="E40" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],7,FALSE)</f>
@@ -5079,7 +5076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -5096,7 +5093,7 @@
       </c>
       <c r="E41" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],7,FALSE)</f>
@@ -5115,7 +5112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -5132,7 +5129,7 @@
       </c>
       <c r="E42" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],7,FALSE)</f>
@@ -5151,7 +5148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -5168,7 +5165,7 @@
       </c>
       <c r="E43" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],7,FALSE)</f>
@@ -5187,7 +5184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -5204,7 +5201,7 @@
       </c>
       <c r="E44" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],7,FALSE)</f>
@@ -5223,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -5240,7 +5237,7 @@
       </c>
       <c r="E45" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="9">
         <f>VLOOKUP(TBL_Ü_S_System[[#This Row],[Schwerpunkt Systemtechnik]],TBL_S_System[#All],7,FALSE)</f>
@@ -5259,7 +5256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>153</v>
       </c>
@@ -5288,7 +5285,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>154</v>
       </c>
@@ -5305,7 +5302,7 @@
       </c>
       <c r="E48" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],7,FALSE)</f>
@@ -5324,7 +5321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>156</v>
       </c>
@@ -5341,7 +5338,7 @@
       </c>
       <c r="E49" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],7,FALSE)</f>
@@ -5360,7 +5357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>157</v>
       </c>
@@ -5377,7 +5374,7 @@
       </c>
       <c r="E50" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],7,FALSE)</f>
@@ -5396,7 +5393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>159</v>
       </c>
@@ -5413,7 +5410,7 @@
       </c>
       <c r="E51" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],7,FALSE)</f>
@@ -5432,7 +5429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>160</v>
       </c>
@@ -5449,7 +5446,7 @@
       </c>
       <c r="E52" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],7,FALSE)</f>
@@ -5468,7 +5465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>161</v>
       </c>
@@ -5485,7 +5482,7 @@
       </c>
       <c r="E53" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],7,FALSE)</f>
@@ -5504,7 +5501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>162</v>
       </c>
@@ -5521,7 +5518,7 @@
       </c>
       <c r="E54" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],7,FALSE)</f>
@@ -5540,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>163</v>
       </c>
@@ -5557,7 +5554,7 @@
       </c>
       <c r="E55" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],7,FALSE)</f>
@@ -5576,7 +5573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>165</v>
       </c>
@@ -5593,7 +5590,7 @@
       </c>
       <c r="E56" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" s="9">
         <f>VLOOKUP(TBL_Ü_S_Software[[#This Row],[Schwerpunkt Softwareentwicklung]],TBL_S_Software[#All],7,FALSE)</f>
@@ -5612,7 +5609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -5632,7 +5629,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>177</v>
       </c>
@@ -5649,14 +5646,14 @@
       </c>
       <c r="E59" s="9">
         <f>VLOOKUP(TBL_Ü_Allgemein[[#This Row],[Allgemeines]],TBL_Allgemeines[#All],5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59" s="9">
         <f>VLOOKUP(TBL_Ü_Allgemein[[#This Row],[Allgemeines]],TBL_Allgemeines[#All],6,FALSE)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>178</v>
       </c>
@@ -5673,14 +5670,14 @@
       </c>
       <c r="E60" s="9">
         <f>VLOOKUP(TBL_Ü_Allgemein[[#This Row],[Allgemeines]],TBL_Allgemeines[#All],5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" s="9">
         <f>VLOOKUP(TBL_Ü_Allgemein[[#This Row],[Allgemeines]],TBL_Allgemeines[#All],6,FALSE)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>179</v>
       </c>
@@ -5697,14 +5694,14 @@
       </c>
       <c r="E61" s="9">
         <f>VLOOKUP(TBL_Ü_Allgemein[[#This Row],[Allgemeines]],TBL_Allgemeines[#All],5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" s="9">
         <f>VLOOKUP(TBL_Ü_Allgemein[[#This Row],[Allgemeines]],TBL_Allgemeines[#All],6,FALSE)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>180</v>
       </c>
@@ -5721,7 +5718,7 @@
       </c>
       <c r="E62" s="9">
         <f>VLOOKUP(TBL_Ü_Allgemein[[#This Row],[Allgemeines]],TBL_Allgemeines[#All],5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" s="9">
         <f>VLOOKUP(TBL_Ü_Allgemein[[#This Row],[Allgemeines]],TBL_Allgemeines[#All],6,FALSE)</f>
@@ -5759,45 +5756,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7F3A44-E98C-4E35-95F6-701F7D50EE0B}">
   <dimension ref="A1:IR55"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.453125" customWidth="1"/>
-    <col min="15" max="46" width="3.453125" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="61" width="3.26953125" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="3.26953125" customWidth="1"/>
-    <col min="63" max="99" width="3.26953125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="100" max="100" width="3.453125" customWidth="1" collapsed="1"/>
-    <col min="101" max="137" width="3.453125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="138" max="138" width="3.453125" customWidth="1" collapsed="1"/>
-    <col min="139" max="175" width="3.453125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="176" max="176" width="3.453125" customWidth="1" collapsed="1"/>
-    <col min="177" max="213" width="3.453125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="214" max="214" width="3.453125" customWidth="1" collapsed="1"/>
-    <col min="215" max="251" width="3.453125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="252" max="252" width="11.453125" collapsed="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.42578125" customWidth="1"/>
+    <col min="15" max="46" width="3.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="61" width="3.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="3.28515625" customWidth="1"/>
+    <col min="63" max="99" width="3.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="100" max="100" width="3.42578125" customWidth="1" collapsed="1"/>
+    <col min="101" max="137" width="3.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="138" max="138" width="3.42578125" customWidth="1" collapsed="1"/>
+    <col min="139" max="175" width="3.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="176" max="176" width="3.42578125" customWidth="1" collapsed="1"/>
+    <col min="177" max="213" width="3.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="214" max="214" width="3.42578125" customWidth="1" collapsed="1"/>
+    <col min="215" max="251" width="3.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="252" max="252" width="11.42578125" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:251" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:251" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:251" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:251" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="N2" s="35" t="s">
         <v>125</v>
       </c>
@@ -6049,7 +6048,7 @@
       <c r="IP2" s="36"/>
       <c r="IQ2" s="37"/>
     </row>
-    <row r="3" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:251" x14ac:dyDescent="0.25">
       <c r="N3" s="10"/>
       <c r="BI3" s="11"/>
       <c r="BJ3" s="10"/>
@@ -6063,7 +6062,7 @@
       <c r="HF3" s="10"/>
       <c r="IQ3" s="11"/>
     </row>
-    <row r="4" spans="1:251" ht="80.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:251" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -6818,7 +6817,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="5" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -6837,8 +6836,8 @@
         <v>8</v>
       </c>
       <c r="F5">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G5">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -6920,7 +6919,7 @@
       <c r="HF5" s="10"/>
       <c r="IQ5" s="11"/>
     </row>
-    <row r="6" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -6939,8 +6938,8 @@
         <v>16</v>
       </c>
       <c r="F6">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G6">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -7016,7 +7015,7 @@
       <c r="HF6" s="10"/>
       <c r="IQ6" s="11"/>
     </row>
-    <row r="7" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -7035,8 +7034,8 @@
         <v>16</v>
       </c>
       <c r="F7">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G7">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -7109,7 +7108,7 @@
       <c r="HF7" s="10"/>
       <c r="IQ7" s="11"/>
     </row>
-    <row r="8" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -7128,8 +7127,8 @@
         <v>8</v>
       </c>
       <c r="F8">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G8">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -7202,7 +7201,7 @@
       <c r="HF8" s="10"/>
       <c r="IQ8" s="11"/>
     </row>
-    <row r="9" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -7221,8 +7220,8 @@
         <v>16</v>
       </c>
       <c r="F9">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G9">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -7295,7 +7294,7 @@
       <c r="HF9" s="10"/>
       <c r="IQ9" s="11"/>
     </row>
-    <row r="10" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -7314,8 +7313,8 @@
         <v>16</v>
       </c>
       <c r="F10">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G10">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -7388,7 +7387,7 @@
       <c r="HF10" s="10"/>
       <c r="IQ10" s="11"/>
     </row>
-    <row r="11" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -7407,8 +7406,8 @@
         <v>8</v>
       </c>
       <c r="F11">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G11">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -7481,7 +7480,7 @@
       <c r="HF11" s="10"/>
       <c r="IQ11" s="11"/>
     </row>
-    <row r="12" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -7500,8 +7499,8 @@
         <v>8</v>
       </c>
       <c r="F12">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G12">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -7574,7 +7573,7 @@
       <c r="HF12" s="10"/>
       <c r="IQ12" s="11"/>
     </row>
-    <row r="13" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>95</v>
       </c>
@@ -7593,8 +7592,8 @@
         <v>8</v>
       </c>
       <c r="F13">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G13">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -7667,7 +7666,7 @@
       <c r="HF13" s="10"/>
       <c r="IQ13" s="11"/>
     </row>
-    <row r="14" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -7686,8 +7685,8 @@
         <v>8</v>
       </c>
       <c r="F14">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G14">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -7760,7 +7759,7 @@
       <c r="HF14" s="10"/>
       <c r="IQ14" s="11"/>
     </row>
-    <row r="15" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -7779,8 +7778,8 @@
         <v>16</v>
       </c>
       <c r="F15">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G15">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -7853,7 +7852,7 @@
       <c r="HF15" s="10"/>
       <c r="IQ15" s="11"/>
     </row>
-    <row r="16" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -7872,8 +7871,8 @@
         <v>16</v>
       </c>
       <c r="F16">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G16">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -7946,7 +7945,7 @@
       <c r="HF16" s="10"/>
       <c r="IQ16" s="11"/>
     </row>
-    <row r="17" spans="1:251" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:251" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -7965,8 +7964,8 @@
         <v>8</v>
       </c>
       <c r="F17">
-        <f>IF(((TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Grundstudium[[#This Row],[LLP Total]]/(TBL_Grundstudium[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G17">
         <f>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</f>
@@ -8219,8 +8218,8 @@
       <c r="IP17" s="15"/>
       <c r="IQ17" s="16"/>
     </row>
-    <row r="18" spans="1:251" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:251" ht="80.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:251" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:251" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -8975,7 +8974,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="20" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -8994,8 +8993,8 @@
         <v>16</v>
       </c>
       <c r="F20">
-        <f>IF(((TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G20">
         <f>TBL_Kommunikation[[#This Row],[Mastery]]+TBL_Kommunikation[[#This Row],[ATL]]+TBL_Kommunikation[[#This Row],[Präsenz]]</f>
@@ -9022,7 +9021,7 @@
       <c r="HF20" s="10"/>
       <c r="IQ20" s="11"/>
     </row>
-    <row r="21" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -9041,8 +9040,8 @@
         <v>16</v>
       </c>
       <c r="F21">
-        <f>IF(((TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G21">
         <f>TBL_Kommunikation[[#This Row],[Mastery]]+TBL_Kommunikation[[#This Row],[ATL]]+TBL_Kommunikation[[#This Row],[Präsenz]]</f>
@@ -9069,7 +9068,7 @@
       <c r="HF21" s="10"/>
       <c r="IQ21" s="11"/>
     </row>
-    <row r="22" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -9088,8 +9087,8 @@
         <v>8</v>
       </c>
       <c r="F22">
-        <f>IF(((TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G22">
         <f>TBL_Kommunikation[[#This Row],[Mastery]]+TBL_Kommunikation[[#This Row],[ATL]]+TBL_Kommunikation[[#This Row],[Präsenz]]</f>
@@ -9116,7 +9115,7 @@
       <c r="HF22" s="10"/>
       <c r="IQ22" s="11"/>
     </row>
-    <row r="23" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -9135,8 +9134,8 @@
         <v>8</v>
       </c>
       <c r="F23">
-        <f>IF(((TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G23">
         <f>TBL_Kommunikation[[#This Row],[Mastery]]+TBL_Kommunikation[[#This Row],[ATL]]+TBL_Kommunikation[[#This Row],[Präsenz]]</f>
@@ -9163,7 +9162,7 @@
       <c r="HF23" s="10"/>
       <c r="IQ23" s="11"/>
     </row>
-    <row r="24" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -9182,8 +9181,8 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <f>IF(((TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G24">
         <f>TBL_Kommunikation[[#This Row],[Mastery]]+TBL_Kommunikation[[#This Row],[ATL]]+TBL_Kommunikation[[#This Row],[Präsenz]]</f>
@@ -9210,7 +9209,7 @@
       <c r="HF24" s="10"/>
       <c r="IQ24" s="11"/>
     </row>
-    <row r="25" spans="1:251" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:251" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -9229,8 +9228,8 @@
         <v>8</v>
       </c>
       <c r="F25">
-        <f>IF(((TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Kommunikation[[#This Row],[LLP Total]]/(TBL_Kommunikation[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G25">
         <f>TBL_Kommunikation[[#This Row],[Mastery]]+TBL_Kommunikation[[#This Row],[ATL]]+TBL_Kommunikation[[#This Row],[Präsenz]]</f>
@@ -9483,8 +9482,8 @@
       <c r="IP25" s="15"/>
       <c r="IQ25" s="16"/>
     </row>
-    <row r="26" spans="1:251" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="27" spans="1:251" ht="80.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:251" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:251" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -10239,7 +10238,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="28" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -10258,8 +10257,8 @@
         <v>16</v>
       </c>
       <c r="F28">
-        <f>IF(((TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G28">
         <f>TBL_S_System[[#This Row],[Mastery]]+TBL_S_System[[#This Row],[ATL]]+TBL_S_System[[#This Row],[Präsenz]]</f>
@@ -10286,7 +10285,7 @@
       <c r="HF28" s="10"/>
       <c r="IQ28" s="11"/>
     </row>
-    <row r="29" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -10305,8 +10304,8 @@
         <v>24</v>
       </c>
       <c r="F29">
-        <f>IF(((TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G29">
         <f>TBL_S_System[[#This Row],[Mastery]]+TBL_S_System[[#This Row],[ATL]]+TBL_S_System[[#This Row],[Präsenz]]</f>
@@ -10333,7 +10332,7 @@
       <c r="HF29" s="10"/>
       <c r="IQ29" s="11"/>
     </row>
-    <row r="30" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -10352,8 +10351,8 @@
         <v>8</v>
       </c>
       <c r="F30">
-        <f>IF(((TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G30">
         <f>TBL_S_System[[#This Row],[Mastery]]+TBL_S_System[[#This Row],[ATL]]+TBL_S_System[[#This Row],[Präsenz]]</f>
@@ -10380,7 +10379,7 @@
       <c r="HF30" s="10"/>
       <c r="IQ30" s="11"/>
     </row>
-    <row r="31" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -10399,8 +10398,8 @@
         <v>8</v>
       </c>
       <c r="F31">
-        <f>IF(((TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G31">
         <f>TBL_S_System[[#This Row],[Mastery]]+TBL_S_System[[#This Row],[ATL]]+TBL_S_System[[#This Row],[Präsenz]]</f>
@@ -10427,7 +10426,7 @@
       <c r="HF31" s="10"/>
       <c r="IQ31" s="11"/>
     </row>
-    <row r="32" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -10446,8 +10445,8 @@
         <v>8</v>
       </c>
       <c r="F32">
-        <f>IF(((TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G32">
         <f>TBL_S_System[[#This Row],[Mastery]]+TBL_S_System[[#This Row],[ATL]]+TBL_S_System[[#This Row],[Präsenz]]</f>
@@ -10474,7 +10473,7 @@
       <c r="HF32" s="10"/>
       <c r="IQ32" s="11"/>
     </row>
-    <row r="33" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -10493,8 +10492,8 @@
         <v>8</v>
       </c>
       <c r="F33">
-        <f>IF(((TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G33">
         <f>TBL_S_System[[#This Row],[Mastery]]+TBL_S_System[[#This Row],[ATL]]+TBL_S_System[[#This Row],[Präsenz]]</f>
@@ -10521,7 +10520,7 @@
       <c r="HF33" s="10"/>
       <c r="IQ33" s="11"/>
     </row>
-    <row r="34" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -10540,8 +10539,8 @@
         <v>8</v>
       </c>
       <c r="F34">
-        <f>IF(((TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G34">
         <f>TBL_S_System[[#This Row],[Mastery]]+TBL_S_System[[#This Row],[ATL]]+TBL_S_System[[#This Row],[Präsenz]]</f>
@@ -10568,7 +10567,7 @@
       <c r="HF34" s="10"/>
       <c r="IQ34" s="11"/>
     </row>
-    <row r="35" spans="1:251" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:251" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -10587,8 +10586,8 @@
         <v>16</v>
       </c>
       <c r="F35">
-        <f>IF(((TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_System[[#This Row],[LLP Total]]/(TBL_S_System[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G35">
         <f>TBL_S_System[[#This Row],[Mastery]]+TBL_S_System[[#This Row],[ATL]]+TBL_S_System[[#This Row],[Präsenz]]</f>
@@ -10841,8 +10840,8 @@
       <c r="IP35" s="15"/>
       <c r="IQ35" s="16"/>
     </row>
-    <row r="36" spans="1:251" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="37" spans="1:251" ht="83.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:251" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:251" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>153</v>
       </c>
@@ -11597,7 +11596,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="38" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>154</v>
       </c>
@@ -11616,8 +11615,8 @@
         <v>8</v>
       </c>
       <c r="F38">
-        <f>IF(((TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G38">
         <f>TBL_S_Software[[#This Row],[Mastery]]+TBL_S_Software[[#This Row],[ATL]]+TBL_S_Software[[#This Row],[Präsenz]]</f>
@@ -11644,7 +11643,7 @@
       <c r="HF38" s="10"/>
       <c r="IQ38" s="11"/>
     </row>
-    <row r="39" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>156</v>
       </c>
@@ -11663,8 +11662,8 @@
         <v>8</v>
       </c>
       <c r="F39">
-        <f>IF(((TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G39">
         <f>TBL_S_Software[[#This Row],[Mastery]]+TBL_S_Software[[#This Row],[ATL]]+TBL_S_Software[[#This Row],[Präsenz]]</f>
@@ -11691,7 +11690,7 @@
       <c r="HF39" s="10"/>
       <c r="IQ39" s="11"/>
     </row>
-    <row r="40" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>157</v>
       </c>
@@ -11710,8 +11709,8 @@
         <v>8</v>
       </c>
       <c r="F40">
-        <f>IF(((TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G40">
         <f>TBL_S_Software[[#This Row],[Mastery]]+TBL_S_Software[[#This Row],[ATL]]+TBL_S_Software[[#This Row],[Präsenz]]</f>
@@ -11738,7 +11737,7 @@
       <c r="HF40" s="10"/>
       <c r="IQ40" s="11"/>
     </row>
-    <row r="41" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>159</v>
       </c>
@@ -11757,8 +11756,8 @@
         <v>24</v>
       </c>
       <c r="F41">
-        <f>IF(((TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G41">
         <f>TBL_S_Software[[#This Row],[Mastery]]+TBL_S_Software[[#This Row],[ATL]]+TBL_S_Software[[#This Row],[Präsenz]]</f>
@@ -11785,7 +11784,7 @@
       <c r="HF41" s="10"/>
       <c r="IQ41" s="11"/>
     </row>
-    <row r="42" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>160</v>
       </c>
@@ -11804,8 +11803,8 @@
         <v>8</v>
       </c>
       <c r="F42">
-        <f>IF(((TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G42">
         <f>TBL_S_Software[[#This Row],[Mastery]]+TBL_S_Software[[#This Row],[ATL]]+TBL_S_Software[[#This Row],[Präsenz]]</f>
@@ -11832,7 +11831,7 @@
       <c r="HF42" s="10"/>
       <c r="IQ42" s="11"/>
     </row>
-    <row r="43" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>161</v>
       </c>
@@ -11851,8 +11850,8 @@
         <v>16</v>
       </c>
       <c r="F43">
-        <f>IF(((TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G43">
         <f>TBL_S_Software[[#This Row],[Mastery]]+TBL_S_Software[[#This Row],[ATL]]+TBL_S_Software[[#This Row],[Präsenz]]</f>
@@ -11879,7 +11878,7 @@
       <c r="HF43" s="10"/>
       <c r="IQ43" s="11"/>
     </row>
-    <row r="44" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>162</v>
       </c>
@@ -11898,8 +11897,8 @@
         <v>8</v>
       </c>
       <c r="F44">
-        <f>IF(((TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G44">
         <f>TBL_S_Software[[#This Row],[Mastery]]+TBL_S_Software[[#This Row],[ATL]]+TBL_S_Software[[#This Row],[Präsenz]]</f>
@@ -11926,7 +11925,7 @@
       <c r="HF44" s="10"/>
       <c r="IQ44" s="11"/>
     </row>
-    <row r="45" spans="1:251" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:251" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>163</v>
       </c>
@@ -11945,8 +11944,8 @@
         <v>8</v>
       </c>
       <c r="F45">
-        <f>IF(((TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G45">
         <f>TBL_S_Software[[#This Row],[Mastery]]+TBL_S_Software[[#This Row],[ATL]]+TBL_S_Software[[#This Row],[Präsenz]]</f>
@@ -11973,7 +11972,7 @@
       <c r="HF45" s="10"/>
       <c r="IQ45" s="11"/>
     </row>
-    <row r="46" spans="1:251" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:251" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>165</v>
       </c>
@@ -11992,8 +11991,8 @@
         <v>8</v>
       </c>
       <c r="F46">
-        <f>IF(((TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_S_Software[[#This Row],[LLP Total]]/(TBL_S_Software[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
       </c>
       <c r="G46">
         <f>TBL_S_Software[[#This Row],[Mastery]]+TBL_S_Software[[#This Row],[ATL]]+TBL_S_Software[[#This Row],[Präsenz]]</f>
@@ -12246,7 +12245,7 @@
       <c r="IP46" s="15"/>
       <c r="IQ46" s="16"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>119</v>
       </c>
@@ -12266,7 +12265,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>177</v>
       </c>
@@ -12280,11 +12279,11 @@
         <v>400</v>
       </c>
       <c r="E50">
-        <f>IF(((TBL_Allgemeines[[#This Row],[LLP Total]]/(TBL_Allgemeines[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Allgemeines[[#This Row],[LLP Total]]/(TBL_Allgemeines[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/((TBL_Allgemeines[[#This Row],[LLP max]]*0.6)-TBL_Allgemeines[[#This Row],[LLP max]]*0.16))*TBL_Allgemeines[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>178</v>
       </c>
@@ -12298,11 +12297,11 @@
         <v>72</v>
       </c>
       <c r="E51">
-        <f>IF(((TBL_Allgemeines[[#This Row],[LLP Total]]/(TBL_Allgemeines[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Allgemeines[[#This Row],[LLP Total]]/(TBL_Allgemeines[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/((TBL_Allgemeines[[#This Row],[LLP max]]*0.6)-TBL_Allgemeines[[#This Row],[LLP max]]*0.16))*TBL_Allgemeines[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>179</v>
       </c>
@@ -12316,11 +12315,11 @@
         <v>600</v>
       </c>
       <c r="E52">
-        <f>IF(((TBL_Allgemeines[[#This Row],[LLP Total]]/(TBL_Allgemeines[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Allgemeines[[#This Row],[LLP Total]]/(TBL_Allgemeines[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/((TBL_Allgemeines[[#This Row],[LLP max]]*0.6)-TBL_Allgemeines[[#This Row],[LLP max]]*0.16))*TBL_Allgemeines[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>180</v>
       </c>
@@ -12334,11 +12333,11 @@
         <v>120</v>
       </c>
       <c r="E53">
-        <f>IF(((TBL_Allgemeines[[#This Row],[LLP Total]]/(TBL_Allgemeines[[#This Row],[LLP max]]*0.9)*5)+1)&gt;=6,6,(TBL_Allgemeines[[#This Row],[LLP Total]]/(TBL_Allgemeines[[#This Row],[LLP max]]*0.9)*5))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/((TBL_Allgemeines[[#This Row],[LLP max]]*0.6)-TBL_Allgemeines[[#This Row],[LLP max]]*0.16))*TBL_Allgemeines[[#This Row],[LLP Total]]))),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -12394,15 +12393,15 @@
       <selection activeCell="A35" sqref="A35:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" customWidth="1"/>
-    <col min="2" max="2" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -12415,7 +12414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -12433,7 +12432,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -12451,7 +12450,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -12469,7 +12468,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -12487,7 +12486,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -12505,7 +12504,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -12523,7 +12522,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -12541,7 +12540,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -12559,7 +12558,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -12577,7 +12576,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -12595,7 +12594,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -12613,7 +12612,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -12631,7 +12630,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -12649,14 +12648,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -12674,7 +12673,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -12692,7 +12691,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -12710,7 +12709,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -12728,7 +12727,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -12746,7 +12745,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -12764,14 +12763,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -12789,7 +12788,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -12807,7 +12806,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -12825,7 +12824,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>98</v>
       </c>
@@ -12843,7 +12842,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -12861,7 +12860,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -12879,7 +12878,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -12897,7 +12896,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -12915,14 +12914,14 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
         <v>153</v>
       </c>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>154</v>
       </c>
@@ -12940,7 +12939,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>156</v>
       </c>
@@ -12958,7 +12957,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -12976,7 +12975,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -12994,7 +12993,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -13012,7 +13011,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>161</v>
       </c>
@@ -13030,7 +13029,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>162</v>
       </c>
@@ -13048,7 +13047,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>163</v>
       </c>
@@ -13066,7 +13065,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>165</v>
       </c>
@@ -13098,14 +13097,14 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>101</v>
       </c>
@@ -13116,7 +13115,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -13127,7 +13126,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -13138,7 +13137,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -13149,7 +13148,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -13160,7 +13159,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -13171,7 +13170,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -13182,10 +13181,10 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>116</v>
       </c>
@@ -13195,169 +13194,169 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
     </row>
   </sheetData>
@@ -13372,17 +13371,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -13390,7 +13389,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -13398,7 +13397,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -13412,12 +13411,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d95b54d8-9ccd-4c6e-b2f5-abf406a92e6e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="184f97ed-d945-4e2b-99fb-8c29b51cdd54">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13616,20 +13617,23 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d95b54d8-9ccd-4c6e-b2f5-abf406a92e6e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="184f97ed-d945-4e2b-99fb-8c29b51cdd54">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E96C37-728E-4F47-9780-7A9362C2741C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A08797BE-B280-492E-A60A-089EB6F53075}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
+    <ds:schemaRef ds:uri="d95b54d8-9ccd-4c6e-b2f5-abf406a92e6e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema-instance"/>
+    <ds:schemaRef ds:uri="184f97ed-d945-4e2b-99fb-8c29b51cdd54"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13655,14 +13659,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A08797BE-B280-492E-A60A-089EB6F53075}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E96C37-728E-4F47-9780-7A9362C2741C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
-    <ds:schemaRef ds:uri="d95b54d8-9ccd-4c6e-b2f5-abf406a92e6e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema-instance"/>
-    <ds:schemaRef ds:uri="184f97ed-d945-4e2b-99fb-8c29b51cdd54"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
:rocket: Update vom 30.03.2023 Mittag
</commit_message>
<xml_diff>
--- a/Kontrolle Noten und Anwesenheit_Template.xlsx
+++ b/Kontrolle Noten und Anwesenheit_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://baumgartnerrhf.sharepoint.com/sites/hfict/Freigegebene Dokumente/01 Allgemeine Informationen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1694" documentId="13_ncr:1_{E46A93A5-8711-4C71-8FC9-6D0FE0D618DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18D3787B-B815-4333-A5CF-0F644F262D75}"/>
+  <xr:revisionPtr revIDLastSave="1704" documentId="13_ncr:1_{E46A93A5-8711-4C71-8FC9-6D0FE0D618DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C9AA082-5CCD-4C46-83E8-6D0274ECBE3D}"/>
   <bookViews>
-    <workbookView xWindow="20235" yWindow="3600" windowWidth="26325" windowHeight="19110" xr2:uid="{0EC385B7-3D0C-45EA-864E-7EE127AA989A}"/>
+    <workbookView xWindow="7365" yWindow="3240" windowWidth="35760" windowHeight="19110" activeTab="1" xr2:uid="{0EC385B7-3D0C-45EA-864E-7EE127AA989A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hauptübersicht" sheetId="3" r:id="rId1"/>
@@ -2440,6 +2440,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3B6417C9-6B84-43EC-8BC6-8A9B7B5F2F54}" name="TBL_Ü_Grund" displayName="TBL_Ü_Grund" ref="A14:I27" totalsRowShown="0">
   <autoFilter ref="A14:I27" xr:uid="{3B6417C9-6B84-43EC-8BC6-8A9B7B5F2F54}"/>
@@ -2481,7 +2485,7 @@
     <tableColumn id="3" xr3:uid="{2618ED18-84F8-40E0-89E6-DBD03E5614F0}" name="Status" dataDxfId="23"/>
     <tableColumn id="4" xr3:uid="{4A77C64F-316A-4D24-9F63-6BD4F2EA8963}" name="LLP max"/>
     <tableColumn id="5" xr3:uid="{BE713E1B-AE97-4051-A260-5B90326948E1}" name="Note" dataDxfId="0">
-      <calculatedColumnFormula>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/((TBL_Allgemeines[[#This Row],[LLP max]]*0.6)-TBL_Allgemeines[[#This Row],[LLP max]]*0.16))*TBL_Allgemeines[[#This Row],[LLP Total]]))),2)</calculatedColumnFormula>
+      <calculatedColumnFormula>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/(TBL_Allgemeines[[#This Row],[LLP max]]*0.6)*TBL_Allgemeines[[#This Row],[LLP Total]])))),2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{E357EBB0-CCB5-4DE1-BB3B-4382AD9C871D}" name="LLP Total"/>
   </tableColumns>
@@ -2503,7 +2507,7 @@
       <calculatedColumnFormula>TBL_S_Software[[#This Row],[Mastery Max]]+TBL_S_Software[[#This Row],[ATL Max]]+TBL_S_Software[[#This Row],[Präsenz Max]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{BF45F161-567C-49D8-89A0-85A89818A93C}" name="Note" dataDxfId="1">
-      <calculatedColumnFormula>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</calculatedColumnFormula>
+      <calculatedColumnFormula>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/(TBL_S_Software[[#This Row],[LLP max]]*0.6)*TBL_S_Software[[#This Row],[LLP Total]])))),2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="23" xr3:uid="{D4002414-1F10-4958-BAAE-615B24C98835}" name="LLP Total" dataDxfId="19">
       <calculatedColumnFormula>TBL_S_Software[[#This Row],[Mastery]]+TBL_S_Software[[#This Row],[ATL]]+TBL_S_Software[[#This Row],[Präsenz]]</calculatedColumnFormula>
@@ -2912,7 +2916,7 @@
       <calculatedColumnFormula>TBL_Grundstudium[[#This Row],[Mastery Max]]+TBL_Grundstudium[[#This Row],[ATL Max]]+TBL_Grundstudium[[#This Row],[Präsenz Max]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="24" xr3:uid="{93B0D6BC-5ADE-4590-A559-7B1578F3979D}" name="Note" dataDxfId="4">
-      <calculatedColumnFormula>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</calculatedColumnFormula>
+      <calculatedColumnFormula>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{1C63CD85-FD5E-4C78-B083-4F597A63F5C9}" name="LLP Total" dataDxfId="122">
       <calculatedColumnFormula>TBL_Grundstudium[[#This Row],[Mastery]]+TBL_Grundstudium[[#This Row],[ATL]]+TBL_Grundstudium[[#This Row],[Präsenz]]</calculatedColumnFormula>
@@ -3186,7 +3190,7 @@
       <calculatedColumnFormula>TBL_Kommunikation[[#This Row],[Mastery Max]]+TBL_Kommunikation[[#This Row],[ATL Max]]+TBL_Kommunikation[[#This Row],[Präsenz Max]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="24" xr3:uid="{C8A9F2E1-E1C8-4CBE-B012-DB7D53BCC34B}" name="Note" dataDxfId="3">
-      <calculatedColumnFormula>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</calculatedColumnFormula>
+      <calculatedColumnFormula>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/(TBL_Kommunikation[[#This Row],[LLP max]]*0.6)*TBL_Kommunikation[[#This Row],[LLP Total]])))),2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DEDF4D39-AB24-42BF-961A-2386150F6639}" name="LLP Total" dataDxfId="56">
       <calculatedColumnFormula>TBL_Kommunikation[[#This Row],[Mastery]]+TBL_Kommunikation[[#This Row],[ATL]]+TBL_Kommunikation[[#This Row],[Präsenz]]</calculatedColumnFormula>
@@ -3458,7 +3462,7 @@
       <calculatedColumnFormula>TBL_S_System[[#This Row],[Mastery Max]]+TBL_S_System[[#This Row],[ATL Max]]+TBL_S_System[[#This Row],[Präsenz Max]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{ECF2CE53-2E14-4BFB-9B0F-74C1B43C8821}" name="Note" dataDxfId="2">
-      <calculatedColumnFormula>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</calculatedColumnFormula>
+      <calculatedColumnFormula>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/(TBL_S_System[[#This Row],[LLP max]]*0.6)*TBL_S_System[[#This Row],[LLP Total]])))),2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="23" xr3:uid="{54181AB0-5314-4A6D-A364-D83146CB91F9}" name="LLP Total" dataDxfId="38">
       <calculatedColumnFormula>TBL_S_System[[#This Row],[Mastery]]+TBL_S_System[[#This Row],[ATL]]+TBL_S_System[[#This Row],[Präsenz]]</calculatedColumnFormula>
@@ -4015,7 +4019,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E379179-39AD-43D4-B056-5A4C09B92C59}">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4065,7 +4071,7 @@
         <v>1368</v>
       </c>
       <c r="E4">
-        <f>IF(SUM(TBL_Ü_Grund[LLP total])&gt;=SUM(TBL_Ü_Grund[LLP max])*0.9,6,IF(SUM(TBL_Ü_Grund[LLP total])&lt;=SUM(TBL_Ü_Grund[LLP max])*0.16,1,IF(SUM(TBL_Ü_Grund[LLP total])&gt;SUM(TBL_Ü_Grund[LLP max])*0.6,(2/((SUM(TBL_Ü_Grund[LLP max])*0.9)-(SUM(TBL_Ü_Grund[LLP max])*0.6))*SUM(TBL_Ü_Grund[LLP total])),(4/((SUM(TBL_Ü_Grund[LLP max])*0.6)-SUM(TBL_Ü_Grund[LLP max])*0.16))*SUM(TBL_Ü_Grund[LLP total]))))</f>
+        <f>IF(SUM(TBL_Ü_Grund[LLP total])&gt;=SUM(TBL_Ü_Grund[LLP max])*0.9,6,IF(SUM(TBL_Ü_Grund[LLP total])&lt;=SUM(TBL_Ü_Grund[LLP max])*0.16,1,IF(SUM(TBL_Ü_Grund[LLP total])&gt;SUM(TBL_Ü_Grund[LLP max])*0.6,(2/((SUM(TBL_Ü_Grund[LLP max])*0.9)-(SUM(TBL_Ü_Grund[LLP max])*0.6))*SUM(TBL_Ü_Grund[LLP total])),(4/(SUM(TBL_Ü_Grund[LLP max])*0.6)*SUM(TBL_Ü_Grund[LLP total])))))</f>
         <v>1</v>
       </c>
     </row>
@@ -4081,7 +4087,7 @@
         <v>576</v>
       </c>
       <c r="E5">
-        <f>IF(SUM(TBL_Ü_Kommunikation[LLP total])&gt;=SUM(TBL_Ü_Kommunikation[LLP max])*0.9,6,IF(SUM(TBL_Ü_Kommunikation[LLP total])&lt;=SUM(TBL_Ü_Kommunikation[LLP max])*0.16,1,IF(SUM(TBL_Ü_Kommunikation[LLP total])&gt;SUM(TBL_Ü_Kommunikation[LLP max])*0.6,(2/((SUM(TBL_Ü_Kommunikation[LLP max])*0.9)-(SUM(TBL_Ü_Kommunikation[LLP max])*0.6))*SUM(TBL_Ü_Kommunikation[LLP total])),(4/((SUM(TBL_Ü_Kommunikation[LLP max])*0.6)-SUM(TBL_Ü_Kommunikation[LLP max])*0.16))*SUM(TBL_Ü_Kommunikation[LLP total]))))</f>
+        <f>IF(SUM(TBL_Ü_Kommunikation[LLP total])&gt;=SUM(TBL_Ü_Kommunikation[LLP max])*0.9,6,IF(SUM(TBL_Ü_Kommunikation[LLP total])&lt;=SUM(TBL_Ü_Kommunikation[LLP max])*0.16,1,IF(SUM(TBL_Ü_Kommunikation[LLP total])&gt;SUM(TBL_Ü_Kommunikation[LLP max])*0.6,(2/((SUM(TBL_Ü_Kommunikation[LLP max])*0.9)-(SUM(TBL_Ü_Kommunikation[LLP max])*0.6))*SUM(TBL_Ü_Kommunikation[LLP total])),(4/((SUM(TBL_Ü_Kommunikation[LLP max])*0.6))*SUM(TBL_Ü_Kommunikation[LLP total])))))</f>
         <v>1</v>
       </c>
     </row>
@@ -4097,7 +4103,7 @@
         <v>864</v>
       </c>
       <c r="E6">
-        <f>IF(SUM(TBL_Ü_S_System[LLP total])&gt;=SUM(TBL_Ü_S_System[LLP max])*0.9,6,IF(SUM(TBL_Ü_S_System[LLP total])&lt;=SUM(TBL_Ü_S_System[LLP max])*0.16,1,IF(SUM(TBL_Ü_S_System[LLP total])&gt;SUM(TBL_Ü_S_System[LLP max])*0.6,(2/((SUM(TBL_Ü_S_System[LLP max])*0.9)-(SUM(TBL_Ü_S_System[LLP max])*0.6))*SUM(TBL_Ü_S_System[LLP total])),(4/((SUM(TBL_Ü_S_System[LLP max])*0.6)-SUM(TBL_Ü_S_System[LLP max])*0.16))*SUM(TBL_Ü_S_System[LLP total]))))</f>
+        <f>IF(SUM(TBL_Ü_S_System[LLP total])&gt;=SUM(TBL_Ü_S_System[LLP max])*0.9,6,IF(SUM(TBL_Ü_S_System[LLP total])&lt;=SUM(TBL_Ü_S_System[LLP max])*0.16,1,IF(SUM(TBL_Ü_S_System[LLP total])&gt;SUM(TBL_Ü_S_System[LLP max])*0.6,(2/((SUM(TBL_Ü_S_System[LLP max])*0.9)-(SUM(TBL_Ü_S_System[LLP max])*0.6))*SUM(TBL_Ü_S_System[LLP total])),(4/((SUM(TBL_Ü_S_System[LLP max])*0.6)*SUM(TBL_Ü_S_System[LLP total]))))))</f>
         <v>1</v>
       </c>
     </row>
@@ -4113,7 +4119,7 @@
         <v>864</v>
       </c>
       <c r="E7">
-        <f>IF(SUM(TBL_Ü_S_Software[LLP total])&gt;=SUM(TBL_Ü_S_Software[LLP max])*0.9,6,IF(SUM(TBL_Ü_S_Software[LLP total])&lt;=SUM(TBL_Ü_S_Software[LLP max])*0.16,1,IF(SUM(TBL_Ü_S_Software[LLP total])&gt;SUM(TBL_Ü_S_Software[LLP max])*0.6,(2/((SUM(TBL_Ü_S_Software[LLP max])*0.9)-(SUM(TBL_Ü_S_Software[LLP max])*0.6))*SUM(TBL_Ü_S_Software[LLP total])),(4/((SUM(TBL_Ü_S_Software[LLP max])*0.6)-SUM(TBL_Ü_S_Software[LLP max])*0.16))*SUM(TBL_Ü_S_Software[LLP total]))))</f>
+        <f>IF(SUM(TBL_Ü_S_Software[LLP total])&gt;=SUM(TBL_Ü_S_Software[LLP max])*0.9,6,IF(SUM(TBL_Ü_S_Software[LLP total])&lt;=SUM(TBL_Ü_S_Software[LLP max])*0.16,1,IF(SUM(TBL_Ü_S_Software[LLP total])&gt;SUM(TBL_Ü_S_Software[LLP max])*0.6,(2/((SUM(TBL_Ü_S_Software[LLP max])*0.9)-(SUM(TBL_Ü_S_Software[LLP max])*0.6))*SUM(TBL_Ü_S_Software[LLP total])),(4/((SUM(TBL_Ü_S_Software[LLP max])*0.6)*SUM(TBL_Ü_S_Software[LLP total]))))))</f>
         <v>1</v>
       </c>
     </row>
@@ -5756,9 +5762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7F3A44-E98C-4E35-95F6-701F7D50EE0B}">
   <dimension ref="A1:IR55"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6836,7 +6840,7 @@
         <v>8</v>
       </c>
       <c r="F5">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G5">
@@ -6938,7 +6942,7 @@
         <v>16</v>
       </c>
       <c r="F6">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G6">
@@ -7034,7 +7038,7 @@
         <v>16</v>
       </c>
       <c r="F7">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G7">
@@ -7127,7 +7131,7 @@
         <v>8</v>
       </c>
       <c r="F8">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G8">
@@ -7220,7 +7224,7 @@
         <v>16</v>
       </c>
       <c r="F9">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G9">
@@ -7313,7 +7317,7 @@
         <v>16</v>
       </c>
       <c r="F10">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G10">
@@ -7406,7 +7410,7 @@
         <v>8</v>
       </c>
       <c r="F11">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G11">
@@ -7499,7 +7503,7 @@
         <v>8</v>
       </c>
       <c r="F12">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G12">
@@ -7592,7 +7596,7 @@
         <v>8</v>
       </c>
       <c r="F13">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G13">
@@ -7685,7 +7689,7 @@
         <v>8</v>
       </c>
       <c r="F14">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G14">
@@ -7778,7 +7782,7 @@
         <v>16</v>
       </c>
       <c r="F15">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G15">
@@ -7871,7 +7875,7 @@
         <v>16</v>
       </c>
       <c r="F16">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G16">
@@ -7964,7 +7968,7 @@
         <v>8</v>
       </c>
       <c r="F17">
-        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)-TBL_Grundstudium[[#This Row],[LLP max]]*0.16))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.9,6,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&lt;=TBL_Grundstudium[[#This Row],[LLP max]]*0.16,1,IF(TBL_Grundstudium[[#This Row],[LLP Total]]&gt;TBL_Grundstudium[[#This Row],[LLP max]]*0.6,(2/((TBL_Grundstudium[[#This Row],[LLP max]]*0.9)-(TBL_Grundstudium[[#This Row],[LLP max]]*0.6))*TBL_Grundstudium[[#This Row],[LLP Total]]),(4/((TBL_Grundstudium[[#This Row],[LLP max]]*0.6)))*TBL_Grundstudium[[#This Row],[LLP Total]]))),2)</f>
         <v>1</v>
       </c>
       <c r="G17">
@@ -8993,7 +8997,7 @@
         <v>16</v>
       </c>
       <c r="F20">
-        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/(TBL_Kommunikation[[#This Row],[LLP max]]*0.6)*TBL_Kommunikation[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G20">
@@ -9040,7 +9044,7 @@
         <v>16</v>
       </c>
       <c r="F21">
-        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/(TBL_Kommunikation[[#This Row],[LLP max]]*0.6)*TBL_Kommunikation[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G21">
@@ -9087,7 +9091,7 @@
         <v>8</v>
       </c>
       <c r="F22">
-        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/(TBL_Kommunikation[[#This Row],[LLP max]]*0.6)*TBL_Kommunikation[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G22">
@@ -9134,7 +9138,7 @@
         <v>8</v>
       </c>
       <c r="F23">
-        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/(TBL_Kommunikation[[#This Row],[LLP max]]*0.6)*TBL_Kommunikation[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G23">
@@ -9181,7 +9185,7 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/(TBL_Kommunikation[[#This Row],[LLP max]]*0.6)*TBL_Kommunikation[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G24">
@@ -9228,7 +9232,7 @@
         <v>8</v>
       </c>
       <c r="F25">
-        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/((TBL_Kommunikation[[#This Row],[LLP max]]*0.6)-TBL_Kommunikation[[#This Row],[LLP max]]*0.16))*TBL_Kommunikation[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.9,6,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&lt;=TBL_Kommunikation[[#This Row],[LLP max]]*0.16,1,IF(TBL_Kommunikation[[#This Row],[LLP Total]]&gt;TBL_Kommunikation[[#This Row],[LLP max]]*0.6,(2/((TBL_Kommunikation[[#This Row],[LLP max]]*0.9)-(TBL_Kommunikation[[#This Row],[LLP max]]*0.6))*TBL_Kommunikation[[#This Row],[LLP Total]]),(4/(TBL_Kommunikation[[#This Row],[LLP max]]*0.6)*TBL_Kommunikation[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G25">
@@ -10257,7 +10261,7 @@
         <v>16</v>
       </c>
       <c r="F28">
-        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/(TBL_S_System[[#This Row],[LLP max]]*0.6)*TBL_S_System[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G28">
@@ -10304,7 +10308,7 @@
         <v>24</v>
       </c>
       <c r="F29">
-        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/(TBL_S_System[[#This Row],[LLP max]]*0.6)*TBL_S_System[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G29">
@@ -10351,7 +10355,7 @@
         <v>8</v>
       </c>
       <c r="F30">
-        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/(TBL_S_System[[#This Row],[LLP max]]*0.6)*TBL_S_System[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G30">
@@ -10398,7 +10402,7 @@
         <v>8</v>
       </c>
       <c r="F31">
-        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/(TBL_S_System[[#This Row],[LLP max]]*0.6)*TBL_S_System[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G31">
@@ -10445,7 +10449,7 @@
         <v>8</v>
       </c>
       <c r="F32">
-        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/(TBL_S_System[[#This Row],[LLP max]]*0.6)*TBL_S_System[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G32">
@@ -10492,7 +10496,7 @@
         <v>8</v>
       </c>
       <c r="F33">
-        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/(TBL_S_System[[#This Row],[LLP max]]*0.6)*TBL_S_System[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G33">
@@ -10539,7 +10543,7 @@
         <v>8</v>
       </c>
       <c r="F34">
-        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/(TBL_S_System[[#This Row],[LLP max]]*0.6)*TBL_S_System[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G34">
@@ -10586,7 +10590,7 @@
         <v>16</v>
       </c>
       <c r="F35">
-        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/((TBL_S_System[[#This Row],[LLP max]]*0.6)-TBL_S_System[[#This Row],[LLP max]]*0.16))*TBL_S_System[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_System[[#This Row],[LLP Total]]&gt;=TBL_S_System[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_System[[#This Row],[LLP Total]]&lt;=TBL_S_System[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_System[[#This Row],[LLP Total]]&gt;TBL_S_System[[#This Row],[LLP max]]*0.6,(2/((TBL_S_System[[#This Row],[LLP max]]*0.9)-(TBL_S_System[[#This Row],[LLP max]]*0.6))*TBL_S_System[[#This Row],[LLP Total]]),(4/(TBL_S_System[[#This Row],[LLP max]]*0.6)*TBL_S_System[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G35">
@@ -11615,7 +11619,7 @@
         <v>8</v>
       </c>
       <c r="F38">
-        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/(TBL_S_Software[[#This Row],[LLP max]]*0.6)*TBL_S_Software[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G38">
@@ -11662,7 +11666,7 @@
         <v>8</v>
       </c>
       <c r="F39">
-        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/(TBL_S_Software[[#This Row],[LLP max]]*0.6)*TBL_S_Software[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G39">
@@ -11709,7 +11713,7 @@
         <v>8</v>
       </c>
       <c r="F40">
-        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/(TBL_S_Software[[#This Row],[LLP max]]*0.6)*TBL_S_Software[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G40">
@@ -11756,7 +11760,7 @@
         <v>24</v>
       </c>
       <c r="F41">
-        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/(TBL_S_Software[[#This Row],[LLP max]]*0.6)*TBL_S_Software[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G41">
@@ -11803,7 +11807,7 @@
         <v>8</v>
       </c>
       <c r="F42">
-        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/(TBL_S_Software[[#This Row],[LLP max]]*0.6)*TBL_S_Software[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G42">
@@ -11850,7 +11854,7 @@
         <v>16</v>
       </c>
       <c r="F43">
-        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/(TBL_S_Software[[#This Row],[LLP max]]*0.6)*TBL_S_Software[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G43">
@@ -11897,7 +11901,7 @@
         <v>8</v>
       </c>
       <c r="F44">
-        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/(TBL_S_Software[[#This Row],[LLP max]]*0.6)*TBL_S_Software[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G44">
@@ -11944,7 +11948,7 @@
         <v>8</v>
       </c>
       <c r="F45">
-        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/(TBL_S_Software[[#This Row],[LLP max]]*0.6)*TBL_S_Software[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G45">
@@ -11991,7 +11995,7 @@
         <v>8</v>
       </c>
       <c r="F46">
-        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/((TBL_S_Software[[#This Row],[LLP max]]*0.6)-TBL_S_Software[[#This Row],[LLP max]]*0.16))*TBL_S_Software[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;=TBL_S_Software[[#This Row],[LLP max]]*0.9,6,IF(TBL_S_Software[[#This Row],[LLP Total]]&lt;=TBL_S_Software[[#This Row],[LLP max]]*0.16,1,IF(TBL_S_Software[[#This Row],[LLP Total]]&gt;TBL_S_Software[[#This Row],[LLP max]]*0.6,(2/((TBL_S_Software[[#This Row],[LLP max]]*0.9)-(TBL_S_Software[[#This Row],[LLP max]]*0.6))*TBL_S_Software[[#This Row],[LLP Total]]),(4/(TBL_S_Software[[#This Row],[LLP max]]*0.6)*TBL_S_Software[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
       <c r="G46">
@@ -12279,7 +12283,7 @@
         <v>400</v>
       </c>
       <c r="E50">
-        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/((TBL_Allgemeines[[#This Row],[LLP max]]*0.6)-TBL_Allgemeines[[#This Row],[LLP max]]*0.16))*TBL_Allgemeines[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/(TBL_Allgemeines[[#This Row],[LLP max]]*0.6)*TBL_Allgemeines[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
     </row>
@@ -12297,7 +12301,7 @@
         <v>72</v>
       </c>
       <c r="E51">
-        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/((TBL_Allgemeines[[#This Row],[LLP max]]*0.6)-TBL_Allgemeines[[#This Row],[LLP max]]*0.16))*TBL_Allgemeines[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/(TBL_Allgemeines[[#This Row],[LLP max]]*0.6)*TBL_Allgemeines[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
     </row>
@@ -12315,7 +12319,7 @@
         <v>600</v>
       </c>
       <c r="E52">
-        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/((TBL_Allgemeines[[#This Row],[LLP max]]*0.6)-TBL_Allgemeines[[#This Row],[LLP max]]*0.16))*TBL_Allgemeines[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/(TBL_Allgemeines[[#This Row],[LLP max]]*0.6)*TBL_Allgemeines[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
     </row>
@@ -12333,7 +12337,7 @@
         <v>120</v>
       </c>
       <c r="E53">
-        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/((TBL_Allgemeines[[#This Row],[LLP max]]*0.6)-TBL_Allgemeines[[#This Row],[LLP max]]*0.16))*TBL_Allgemeines[[#This Row],[LLP Total]]))),2)</f>
+        <f>ROUND(IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.9,6,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&lt;=TBL_Allgemeines[[#This Row],[LLP max]]*0.16,1,IF(TBL_Allgemeines[[#This Row],[LLP Total]]&gt;TBL_Allgemeines[[#This Row],[LLP max]]*0.6,(2/((TBL_Allgemeines[[#This Row],[LLP max]]*0.9)-(TBL_Allgemeines[[#This Row],[LLP max]]*0.6))*TBL_Allgemeines[[#This Row],[LLP Total]]),(4/(TBL_Allgemeines[[#This Row],[LLP max]]*0.6)*TBL_Allgemeines[[#This Row],[LLP Total]])))),2)</f>
         <v>1</v>
       </c>
     </row>
@@ -13411,17 +13415,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d95b54d8-9ccd-4c6e-b2f5-abf406a92e6e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="184f97ed-d945-4e2b-99fb-8c29b51cdd54">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007AF75EAFE5D605439CFC7B6C9FA95DA5" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="76175cbe8591f714e5c1f1cadcd5ca43">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="184f97ed-d945-4e2b-99fb-8c29b51cdd54" xmlns:ns3="d95b54d8-9ccd-4c6e-b2f5-abf406a92e6e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4dd33e8068e1c89cf004524faa747ca7" ns2:_="" ns3:_="">
     <xsd:import namespace="184f97ed-d945-4e2b-99fb-8c29b51cdd54"/>
@@ -13616,6 +13609,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d95b54d8-9ccd-4c6e-b2f5-abf406a92e6e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="184f97ed-d945-4e2b-99fb-8c29b51cdd54">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -13626,19 +13630,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A08797BE-B280-492E-A60A-089EB6F53075}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
-    <ds:schemaRef ds:uri="d95b54d8-9ccd-4c6e-b2f5-abf406a92e6e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema-instance"/>
-    <ds:schemaRef ds:uri="184f97ed-d945-4e2b-99fb-8c29b51cdd54"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62E31675-7B08-4F83-935B-ABFBFF9466C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13658,6 +13649,19 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A08797BE-B280-492E-A60A-089EB6F53075}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
+    <ds:schemaRef ds:uri="d95b54d8-9ccd-4c6e-b2f5-abf406a92e6e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema-instance"/>
+    <ds:schemaRef ds:uri="184f97ed-d945-4e2b-99fb-8c29b51cdd54"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E96C37-728E-4F47-9780-7A9362C2741C}">
   <ds:schemaRefs>

</xml_diff>